<commit_message>
Added MET cutoffs for intensity classes
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -294,22 +294,636 @@
     <t>Time of auto or manually defined non-wear (NW) during the day</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The time within ValidDuration of this calendar day which is </t>
-    </r>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Cadence related variables. Cadence is only detected for walking, running and stair-walking</t>
+  </si>
+  <si>
+    <t>Only available when work/leisure diary is given</t>
+  </si>
+  <si>
+    <t>Important Note: These variables are calculated using the direct output of activity detection algorithm with an epoch of 1s. Any sporadic break, misclassification or ambiguity can affect these variables. These variables, except for the combined activity/posture "SitLie", should only be used with consultation of ActiPASS developers</t>
+  </si>
+  <si>
+    <t>replace "SitLie" with the relevant activity/posture/intensity-class to derive corresponding variable name (also see warning above)</t>
+  </si>
+  <si>
+    <t>Important Note: If ProPASS default settings are applied, then these variables are calculated allowing a fixed bout-break of 20s with 0% bout thresholds. 
+However, if bout-calculations options are changed under advanced settings, different bout-break lengths and different bout-thresholds can be selected. Before generating these variables make sure desired settings are applied under ActiPASS advanced options</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 1min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 2min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 3min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 4min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 5min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 10min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 30min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts  equal or larger than 60min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 1 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 2 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 3 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 4 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 5 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 10 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 30 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts larger than 60 min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 1min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 2min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 3min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 4min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 5min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 10min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 30min</t>
+  </si>
+  <si>
+    <t>Time spent on SitLie bouts smaller than 60min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 2 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 3 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 4 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 5 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 10 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 30 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 60 min</t>
+  </si>
+  <si>
+    <t>Frequency (count) of SitLie bouts smaller than 1 min</t>
+  </si>
+  <si>
+    <t>replace "SitLie" with the relevant activity/posture/intensity-class to derive corresponding variable name (also see notice above)</t>
+  </si>
+  <si>
+    <t>A day can be further sub-divided into domains such as 'Work' and 'Leisure' and following variables can be generated for each such sub-domain within a calendar day.  Such variables will be prefixed with the domain (Ex. Work_Duration_1) This additional domain specific data is available only when the additional diary containing such data is included in ActiPASS processing, and also the relevant domain names are specified under "Stat Domains" options before stats generation.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>not flagged as belonging to a sleep-interval</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The  time within ValidDuration of this calendar day which is flagged as</t>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Activity/Posture times and cadence related variables. These variables are defined within "Awake". All times are given in minutes. These variables satisfy the equation:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Awake=Lie+Sit+Stand+Move+Walk+Run+Stair+Cycle+Other</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Variables related to the bedtime, sleep-interval and awake time. All times are given in minutes. These variables satisfy the equation:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ValidDuration = Awake + SleepInterval</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Variables related to exclusions, non-wear and validity. All times are given in minutes. These variables satisfy the equations: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Duration = Excluded + NonWear + ValidDuration
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NonWear = AwakeNW +  SlpIntNW
+</t>
+    </r>
+  </si>
+  <si>
+    <t>SitLie_1min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_freq_L_1</t>
+  </si>
+  <si>
+    <t> Intensity class name</t>
+  </si>
+  <si>
+    <t>INT1_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as sedentary on day 1</t>
+  </si>
+  <si>
+    <t>INT2_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as low physical activity on day 1</t>
+  </si>
+  <si>
+    <t>INT2_Amb_1</t>
+  </si>
+  <si>
+    <t>Time spent on ambulatory activities classified as low physical activity  (standing excluded) on day 1</t>
+  </si>
+  <si>
+    <t>INT3_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as moderate physical activity on day 1</t>
+  </si>
+  <si>
+    <t>"Sit" and "Lie"</t>
+  </si>
+  <si>
+    <t>"Stand", "Move", "Walk_Slow" (walking with a cadence lower than 100/min), and "Other" with no periodic movements and "Other" with periodic movements with a cadence lower than 100/min)</t>
+  </si>
+  <si>
+    <t>"Move", "Walk_Slow" (walking with a cadence lower than 100/min), "Other" with no periodic movements, and "Other" with periodic movements with a cadence lower than 100/min)</t>
+  </si>
+  <si>
+    <t>INT4_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as vigorous  physical activity on day 1</t>
+  </si>
+  <si>
+    <t>INT34_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as moderate and vigorous  physical activity on day 1</t>
+  </si>
+  <si>
+    <t>"INT3" and "INT4"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time spent on different energy expenditure intensity classes </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The posture </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"SitLie"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
+    </r>
+  </si>
+  <si>
+    <t>How times are derived</t>
+  </si>
+  <si>
+    <t>Please see following publications for more info about cadence cutoffs for intensity classes</t>
+  </si>
+  <si>
+    <t>"Walk" (with a cadence between 100-135/min) and "Other" with periodic movements with a cadence between 100-135/min</t>
+  </si>
+  <si>
+    <t>"Run", "Cycle", "Stair", "Walk" with a cadence higher than 135/min , "Other" with periodic movement with a cadence higher than or equal to 135/min</t>
+  </si>
+  <si>
+    <t>LieStill_1</t>
+  </si>
+  <si>
+    <t>The total time of possible sleep outside a bedtime (this is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes.). In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
+  </si>
+  <si>
+    <t>Time of lying. If LieStill is defined, time of 'Lie' also contains that time.</t>
+  </si>
+  <si>
+    <t>Total sleep time within ValidDuration of this calendar day</t>
+  </si>
+  <si>
+    <t>ActiPASS Version 1.50 (or higher) Variable Definitions</t>
+  </si>
+  <si>
+    <r>
+      <t>The time of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> NW outside any periods flagged as sleep-intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> not a part of Awake_1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>variable below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The time of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> NW inside any periods flagged as sleep-intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not a part of SleepInterval_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The  time </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>within ValidDuration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of this calendar day which is flagged as</t>
     </r>
     <r>
       <rPr>
@@ -331,136 +945,25 @@
     </r>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Cadence related variables. Cadence is only detected for walking, running and stair-walking</t>
-  </si>
-  <si>
-    <t>Only available when work/leisure diary is given</t>
-  </si>
-  <si>
-    <t>Important Note: These variables are calculated using the direct output of activity detection algorithm with an epoch of 1s. Any sporadic break, misclassification or ambiguity can affect these variables. These variables, except for the combined activity/posture "SitLie", should only be used with consultation of ActiPASS developers</t>
-  </si>
-  <si>
-    <t>replace "SitLie" with the relevant activity/posture/intensity-class to derive corresponding variable name (also see warning above)</t>
-  </si>
-  <si>
-    <t>Important Note: If ProPASS default settings are applied, then these variables are calculated allowing a fixed bout-break of 20s with 0% bout thresholds. 
-However, if bout-calculations options are changed under advanced settings, different bout-break lengths and different bout-thresholds can be selected. Before generating these variables make sure desired settings are applied under ActiPASS advanced options</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 1min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 2min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 3min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 4min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 5min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 10min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 30min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts  equal or larger than 60min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 1 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 2 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 3 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 4 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 5 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 10 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 30 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts larger than 60 min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 1min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 2min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 3min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 4min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 5min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 10min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 30min</t>
-  </si>
-  <si>
-    <t>Time spent on SitLie bouts smaller than 60min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 2 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 3 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 4 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 5 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 10 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 30 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 60 min</t>
-  </si>
-  <si>
-    <t>Frequency (count) of SitLie bouts smaller than 1 min</t>
-  </si>
-  <si>
-    <t>replace "SitLie" with the relevant activity/posture/intensity-class to derive corresponding variable name (also see notice above)</t>
-  </si>
-  <si>
-    <t>A day can be further sub-divided into domains such as 'Work' and 'Leisure' and following variables can be generated for each such sub-domain within a calendar day.  Such variables will be prefixed with the domain (Ex. Work_Duration_1) This additional domain specific data is available only when the additional diary containing such data is included in ActiPASS processing, and also the relevant domain names are specified under "Stat Domains" options before stats generation.</t>
-  </si>
-  <si>
+    <r>
+      <t>The time</t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Activity/Posture times and cadence related variables. These variables are defined within "Awake". All times are given in minutes. These variables satisfy the equation:  </t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> within ValidDuration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of this calendar day which is </t>
     </r>
     <r>
       <rPr>
@@ -469,448 +972,35 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">                      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Awake=Lie+Sit+Stand+Move+Walk+Run+Stair+Cycle+Other</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Variables related to the bedtime, sleep-interval and awake time. All times are given in minutes. These variables satisfy the equation:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ValidDuration = Awake + SleepInterval</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Variables related to exclusions, non-wear and validity. All times are given in minutes. These variables satisfy the equations: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Duration = Excluded + NonWear + ValidDuration
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">NonWear = AwakeNW +  SlpIntNW
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The time of NW </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>outside</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The time of NW </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>inside</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
-    </r>
-  </si>
-  <si>
-    <t>SitLie_1min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_freq_L_1</t>
-  </si>
-  <si>
-    <t> Intensity class name</t>
-  </si>
-  <si>
-    <t>INT1_1</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as sedentary on day 1</t>
-  </si>
-  <si>
-    <t>INT2_1</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as low physical activity on day 1</t>
-  </si>
-  <si>
-    <t>INT2_Amb_1</t>
-  </si>
-  <si>
-    <t>Time spent on ambulatory activities classified as low physical activity  (standing excluded) on day 1</t>
-  </si>
-  <si>
-    <t>INT3_1</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as moderate physical activity on day 1</t>
-  </si>
-  <si>
-    <t>"Sit" and "Lie"</t>
-  </si>
-  <si>
-    <t>"Stand", "Move", "Walk_Slow" (walking with a cadence lower than 100/min), and "Other" with no periodic movements and "Other" with periodic movements with a cadence lower than 100/min)</t>
-  </si>
-  <si>
-    <t>"Move", "Walk_Slow" (walking with a cadence lower than 100/min), "Other" with no periodic movements, and "Other" with periodic movements with a cadence lower than 100/min)</t>
-  </si>
-  <si>
-    <t>INT4_1</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as vigorous  physical activity on day 1</t>
-  </si>
-  <si>
-    <t>INT34_1</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as moderate and vigorous  physical activity on day 1</t>
-  </si>
-  <si>
-    <t>"INT3" and "INT4"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time spent on different energy expenditure intensity classes </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The posture </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"SitLie"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
-    </r>
-  </si>
-  <si>
-    <t>How times are derived</t>
-  </si>
-  <si>
-    <t>Please see following publications for more info about cadence cutoffs for intensity classes</t>
-  </si>
-  <si>
-    <t>Influence of Anthropometrics on Step-Rate Thresholds for Moderate and Vigorous Physical Activity in Older Adults: Scientific Modeling Study
+      <t>not flagged as belonging to a sleep-interval</t>
+    </r>
+  </si>
+  <si>
+    <t>References:
+Influence of Anthropometrics on Step-Rate Thresholds for Moderate and Vigorous Physical Activity in Older Adults: Scientific Modeling Study
 DOI: 10.2196/12363
-Tudor-Locke C, Han H, Aguiar EJ, et alHow fast is fast enough? Walking cadence (steps/min) as a practical estimate of intensity in adults: a narrative reviewBritish Journal of Sports Medicine 2018;52:776-788.</t>
-  </si>
-  <si>
-    <t>"Walk" (with a cadence between 100-135/min) and "Other" with periodic movements with a cadence between 100-135/min</t>
-  </si>
-  <si>
-    <t>"Run", "Cycle", "Stair", "Walk" with a cadence higher than 135/min , "Other" with periodic movement with a cadence higher than or equal to 135/min</t>
-  </si>
-  <si>
-    <t>LieStill_1</t>
-  </si>
-  <si>
-    <t>The total time of possible sleep outside a bedtime (this is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes.). In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
-  </si>
-  <si>
-    <t>Time of lying. If LieStill is defined, time of 'Lie' also contains that time.</t>
-  </si>
-  <si>
-    <t>Total sleep time within ValidDuration of this calendar day</t>
-  </si>
-  <si>
-    <t>ActiPASS Version 1.50 Variable Definitions</t>
+Tudor-Locke C, Han H, Aguiar EJ, et alHow fast is fast enough? Walking cadence (steps/min) as a practical estimate of intensity in adults: a narrative reviewBritish Journal of Sports Medicine 2018;52:776-788.
+% activity to MET translation (these values are used to give each-epoch an equivalent 'MET' value. In other words we create a continuous variable with a resolution of 1s
+Settings.MET_SI=0.90;
+Settings.MET_LieStill=0.95;
+Settings.MET_Lie=1.0;
+Settings.MET_Sit=1.3;
+Settings.MET_Stand=1.55;
+Settings.MET_Move=2.0;
+Settings.Wlk_Low_MET=2;
+Settings.Wlk_Fast_MET=4;
+Settings.Wlk_VFast_MET=7;
+Settings.MET_Running=10;
+Settings.MET_Stairs=8;
+Settings.MET_Cycle=7;
+Settings.MET_Other=2; % "Other" with no periodicity falls into light physical activity and given a fixed MET value of 2, "Other" with periodicity as classified similar to Walk.
+% Then above continuous variable is discretized back into the categorical intensity classes given below with given cutoffs
+Settings.PA_Slp=0.0;
+Settings.PA_SED=0.95;  % lieStill belongs to sedentary
+Settings.PA_LPA=1.5;
+Settings.PA_LPA_Amb=1.6; %introduce another called LPA_ambulatory to seperate standing from other LPA activities
+Settings.PA_MPA=3.0;
+Settings.PA_VPA=6.0;</t>
   </si>
 </sst>
 </file>
@@ -1531,17 +1621,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="3" width="79" style="3" customWidth="1"/>
+    <col min="2" max="2" width="79" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="30" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="30" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1555,7 +1648,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30.75" thickTop="1">
@@ -1610,7 +1703,7 @@
         <v>76</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
@@ -1621,7 +1714,7 @@
         <v>77</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1694,7 +1787,7 @@
     </row>
     <row r="20" spans="1:3" s="15" customFormat="1" ht="90">
       <c r="B20" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C20" s="16"/>
     </row>
@@ -1704,7 +1797,7 @@
     </row>
     <row r="22" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
       <c r="B22" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -1735,21 +1828,21 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="45">
       <c r="A26" t="s">
         <v>88</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="30">
+    <row r="27" spans="1:3" ht="45">
       <c r="A27" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="C27" s="4"/>
     </row>
@@ -1764,7 +1857,7 @@
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
       <c r="B29" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C29" s="6"/>
     </row>
@@ -1773,7 +1866,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="C30" s="10"/>
     </row>
@@ -1782,7 +1875,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="C31" s="10"/>
     </row>
@@ -1791,7 +1884,7 @@
         <v>20</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C32" s="4"/>
     </row>
@@ -1806,15 +1899,15 @@
     </row>
     <row r="34" spans="1:3" ht="45">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
       <c r="B35" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C35" s="6"/>
     </row>
@@ -1823,7 +1916,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -1935,92 +2028,92 @@
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1">
       <c r="C49" s="23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="5" customFormat="1">
       <c r="B50" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="90.75" thickBot="1">
+    </row>
+    <row r="51" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
       <c r="A51" s="26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B51" s="27" t="s">
         <v>46</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="45">
       <c r="A53" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="45">
       <c r="A54" s="28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="30">
       <c r="A55" s="28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="30">
       <c r="A56" s="28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="5" customFormat="1">
       <c r="A57" s="28" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
@@ -2030,7 +2123,7 @@
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1">
       <c r="B59" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2059,15 +2152,15 @@
     </row>
     <row r="65" spans="1:3" s="5" customFormat="1" ht="120">
       <c r="B65" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="C66" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2144,299 +2237,299 @@
     </row>
     <row r="77" spans="1:3" s="5" customFormat="1" ht="90">
       <c r="B77" s="24" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C80" s="34"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C81" s="34"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C82" s="34"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C83" s="34"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C84" s="34"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C85" s="34"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C86" s="34"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C87" s="34"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C88" s="34"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C89" s="34"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C96" s="34"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C97" s="34"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C98" s="34"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C99" s="34"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C100" s="34"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C101" s="34"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C102" s="34"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C103" s="34"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C104" s="34"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C105" s="34"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C106" s="34"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C107" s="34"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C108" s="34"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C109" s="34"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C110" s="34"/>
     </row>

</xml_diff>

<commit_message>
added daily qc variables to variable definitions
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasan\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46B1693-28CE-4F22-A155-4E723B0A2E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="12090"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="222">
   <si>
     <t>varNames</t>
   </si>
@@ -1002,11 +1003,77 @@
   <si>
     <t>Number of work days detected. A work day is a day where some time of the day is flagged as "Work" by  diary. Not available for ProPASS tables.</t>
   </si>
+  <si>
+    <t>Day_QC_1</t>
+  </si>
+  <si>
+    <t>NotEnoughWear_1</t>
+  </si>
+  <si>
+    <t>NoWlk_1</t>
+  </si>
+  <si>
+    <t>TooMuchOther_1</t>
+  </si>
+  <si>
+    <t>TooMuchStair_1</t>
+  </si>
+  <si>
+    <t>NoSleepInt_1</t>
+  </si>
+  <si>
+    <t>NumPrimaryBDs_1</t>
+  </si>
+  <si>
+    <t>NumExtraBDs_1</t>
+  </si>
+  <si>
+    <t>The auto detected quality check flag for the day. ProPASS wide-format table contains days only days where this flag is "OK"</t>
+  </si>
+  <si>
+    <t>A flag indicating if the day has less than 30s of walking</t>
+  </si>
+  <si>
+    <t>When a day has not enough walking, it affects the individual calibration (refrence-positions) and it can then lead to less accurate classifications</t>
+  </si>
+  <si>
+    <t>A flag indicating if the day has not enough wear time (20 hrs). Should always be 0 under ProPASS mode</t>
+  </si>
+  <si>
+    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then it's a problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A flag indicating if more than 30 minutes of "other" exist in the day </t>
+  </si>
+  <si>
+    <t>A flag indicating more than 120 minutes of stair-walking present in the day.</t>
+  </si>
+  <si>
+    <t>Too much stair walking most probably means walking/hiking in steep hills,  confusion with bicycling (somewhat rare but possible) etc.</t>
+  </si>
+  <si>
+    <t>A sleep-interval (a mid-point of a sleep interval to be precise) is not found within the day</t>
+  </si>
+  <si>
+    <t>This is not necessarily a problem. If the missing sleep is a technical problem, this day will then have much higher sedentary times than the other days</t>
+  </si>
+  <si>
+    <t>Number of primary bedtimes (mid points) found within the current day</t>
+  </si>
+  <si>
+    <t>Number of possible extra bedtimes found within the current day</t>
+  </si>
+  <si>
+    <t>Sleep algorithms is used only within these primary bedtimes</t>
+  </si>
+  <si>
+    <t>Slepp algorithm is not used for extra bedtimes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16">
     <font>
       <sz val="11"/>
@@ -1329,6 +1396,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1337,9 +1407,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1625,29 +1692,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.1328125" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.73046875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="29" customFormat="1" ht="19.899999999999999" thickBot="1">
+    <row r="1" spans="1:3" s="29" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="29" t="s">
         <v>192</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
-    <row r="2" spans="1:3" ht="14.65" thickTop="1"/>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="17.25" thickBot="1">
+    <row r="2" spans="1:3" ht="15" thickTop="1"/>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1725,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.9" thickTop="1">
+    <row r="4" spans="1:3" ht="29.4" thickTop="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1666,7 +1733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.5">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1684,7 +1751,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="28.5">
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1702,22 +1769,22 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.5">
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="31" t="s">
         <v>199</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.5">
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="31" t="s">
         <v>198</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1728,7 +1795,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" s="18" customFormat="1" ht="42.75">
+    <row r="12" spans="1:3" s="18" customFormat="1" ht="57.6">
       <c r="B12" s="20" t="s">
         <v>78</v>
       </c>
@@ -1761,7 +1828,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="28.5">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1788,762 +1855,846 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="4"/>
+    <row r="19" spans="1:3" ht="28.8">
+      <c r="A19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>208</v>
+      </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" s="14" customFormat="1" ht="85.5">
-      <c r="B20" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" s="14" customFormat="1">
-      <c r="B21" s="16"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B22" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="6"/>
+    <row r="20" spans="1:3" ht="28.8">
+      <c r="A20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8">
+      <c r="A22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>204</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>205</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" ht="42.75">
+        <v>206</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" ht="42.75">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>194</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B29" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" ht="28.5">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" ht="85.5">
+    <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
+      <c r="B28" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" spans="1:3" s="14" customFormat="1">
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
+      <c r="B30" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>191</v>
+        <v>15</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="28.5">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="42.75">
+    <row r="34" spans="1:3" ht="43.2">
       <c r="A34" t="s">
-        <v>188</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B35" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" ht="43.2">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>190</v>
+        <v>17</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:3">
+    <row r="37" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
+      <c r="B37" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" ht="28.8">
       <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="86.4">
       <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" ht="42.75">
+        <v>19</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>81</v>
+        <v>20</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>191</v>
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="28.8">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="43.2">
       <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
+      <c r="B43" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" ht="43.2">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3" ht="45.75" customHeight="1">
-      <c r="A48" t="s">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" ht="45.75" customHeight="1">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" s="5" customFormat="1">
-      <c r="C49" s="22" t="s">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" s="5" customFormat="1">
+      <c r="C57" s="22" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1">
-      <c r="B50" s="22" t="s">
+    <row r="58" spans="1:3" s="5" customFormat="1">
+      <c r="B58" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
-      <c r="A51" s="25" t="s">
+    <row r="59" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
+      <c r="A59" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B59" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C59" s="26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="27" t="s">
+    <row r="60" spans="1:3">
+      <c r="A60" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B60" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C60" s="28" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="28.5">
-      <c r="A53" s="27" t="s">
+    <row r="61" spans="1:3" ht="28.8">
+      <c r="A61" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B61" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C61" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="28.5">
-      <c r="A54" s="27" t="s">
+    <row r="62" spans="1:3" ht="28.8">
+      <c r="A62" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B62" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C62" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="27" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B63" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C63" s="28" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="27" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B64" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C64" s="28" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1">
-      <c r="A57" s="27" t="s">
+    <row r="65" spans="1:3" s="5" customFormat="1">
+      <c r="A65" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B65" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C65" s="28" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1">
-      <c r="A58" s="27"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-    </row>
-    <row r="59" spans="1:3" s="5" customFormat="1">
-      <c r="B59" s="21" t="s">
+    <row r="66" spans="1:3" s="5" customFormat="1">
+      <c r="A66" s="27"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+    </row>
+    <row r="67" spans="1:3" s="5" customFormat="1">
+      <c r="B67" s="21" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="99.75">
-      <c r="B65" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="C66" s="31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="32"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" s="32"/>
+        <v>24</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>32</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="32"/>
+        <v>25</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="100.8">
+      <c r="B73" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="C74" s="32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="33"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="33"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>32</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C77" s="33"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C70" s="32"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>34</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="32"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" s="32"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>36</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" s="32"/>
-    </row>
-    <row r="74" spans="1:3" ht="28.5">
-      <c r="A74" t="s">
-        <v>37</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C74" s="32"/>
-    </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="71.25">
-      <c r="B77" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C77" s="24" t="s">
-        <v>94</v>
-      </c>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>132</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C79" s="33" t="s">
-        <v>127</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C79" s="33"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>96</v>
+        <v>35</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C80" s="33"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>134</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>97</v>
+        <v>36</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C81" s="33"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" ht="28.8">
       <c r="A82" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>98</v>
+        <v>37</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C82" s="33"/>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>136</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83" s="33"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>137</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C84" s="33"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>138</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="33"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>139</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C86" s="33"/>
+    <row r="85" spans="1:3" s="5" customFormat="1" ht="72">
+      <c r="B85" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>147</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C87" s="33"/>
+        <v>132</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="34" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>140</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C88" s="33"/>
+        <v>133</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C88" s="34"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C89" s="33"/>
+        <v>134</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" s="34"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>142</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C90" s="33"/>
+        <v>135</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>143</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C91" s="33"/>
+        <v>136</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C92" s="33"/>
+        <v>137</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>145</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C93" s="33"/>
+        <v>138</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>146</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C94" s="33"/>
+        <v>139</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>148</v>
-      </c>
-      <c r="B95" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C95" s="33"/>
+        <v>147</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>149</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C96" s="33"/>
+        <v>140</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" s="34"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>150</v>
-      </c>
-      <c r="B97" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C97" s="33"/>
+        <v>141</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C97" s="34"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>151</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C98" s="33"/>
+        <v>142</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="34"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>152</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C99" s="33"/>
+        <v>143</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="34"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>153</v>
-      </c>
-      <c r="B100" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C100" s="33"/>
+        <v>144</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" s="34"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>154</v>
-      </c>
-      <c r="B101" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C101" s="33"/>
+        <v>145</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C101" s="34"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>155</v>
-      </c>
-      <c r="B102" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C102" s="33"/>
+        <v>146</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C102" s="34"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>156</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C103" s="33"/>
+        <v>148</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" s="34"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>157</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C104" s="33"/>
+        <v>149</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C104" s="34"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>158</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C105" s="33"/>
+        <v>150</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C105" s="34"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>159</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C106" s="33"/>
+        <v>151</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C106" s="34"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>160</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C107" s="33"/>
+        <v>152</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" s="34"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>161</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C108" s="33"/>
+        <v>153</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C108" s="34"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>162</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C109" s="33"/>
+        <v>154</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C109" s="34"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" s="34"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>156</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C111" s="34"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>157</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C112" s="34"/>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>158</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113" s="34"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>159</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C114" s="34"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>160</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="34"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>161</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C116" s="34"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>162</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C117" s="34"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
         <v>163</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C110" s="33"/>
+      <c r="C118" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C66:C74"/>
-    <mergeCell ref="C79:C110"/>
+    <mergeCell ref="C74:C82"/>
+    <mergeCell ref="C87:C118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
minor changes to variable definitions doc
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
   <si>
     <t>varNames</t>
   </si>
@@ -797,9 +797,6 @@
     <t>How times are derived</t>
   </si>
   <si>
-    <t>Please see following publications for more info about cadence cutoffs for intensity classes</t>
-  </si>
-  <si>
     <t>"Walk" (with a cadence between 100-135/min) and "Other" with periodic movements with a cadence between 100-135/min</t>
   </si>
   <si>
@@ -970,10 +967,87 @@
     </r>
   </si>
   <si>
+    <t>Number of leisure days detected. A leisure day is where some or whole part of the day is flagged as leisure, but not as work. Not available for ProPASS tables.</t>
+  </si>
+  <si>
+    <t>Number of work days detected. A work day is a day where some time of the day is flagged as "Work" by  diary. Not available for ProPASS tables.</t>
+  </si>
+  <si>
+    <t>Day_QC_1</t>
+  </si>
+  <si>
+    <t>NotEnoughWear_1</t>
+  </si>
+  <si>
+    <t>NoWlk_1</t>
+  </si>
+  <si>
+    <t>TooMuchOther_1</t>
+  </si>
+  <si>
+    <t>TooMuchStair_1</t>
+  </si>
+  <si>
+    <t>NoSleepInt_1</t>
+  </si>
+  <si>
+    <t>NumPrimaryBDs_1</t>
+  </si>
+  <si>
+    <t>NumExtraBDs_1</t>
+  </si>
+  <si>
+    <t>The auto detected quality check flag for the day. ProPASS wide-format table contains days only days where this flag is "OK"</t>
+  </si>
+  <si>
+    <t>A flag indicating if the day has less than 30s of walking</t>
+  </si>
+  <si>
+    <t>When a day has not enough walking, it affects the individual calibration (refrence-positions) and it can then lead to less accurate classifications</t>
+  </si>
+  <si>
+    <t>A flag indicating if the day has not enough wear time (20 hrs). Should always be 0 under ProPASS mode</t>
+  </si>
+  <si>
+    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then it's a problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A flag indicating if more than 30 minutes of "other" exist in the day </t>
+  </si>
+  <si>
+    <t>A flag indicating more than 120 minutes of stair-walking present in the day.</t>
+  </si>
+  <si>
+    <t>Too much stair walking most probably means walking/hiking in steep hills,  confusion with bicycling (somewhat rare but possible) etc.</t>
+  </si>
+  <si>
+    <t>A sleep-interval (a mid-point of a sleep interval to be precise) is not found within the day</t>
+  </si>
+  <si>
+    <t>This is not necessarily a problem. If the missing sleep is a technical problem, this day will then have much higher sedentary times than the other days</t>
+  </si>
+  <si>
+    <t>Number of primary bedtimes (mid points) found within the current day</t>
+  </si>
+  <si>
+    <t>Number of possible extra bedtimes found within the current day</t>
+  </si>
+  <si>
+    <t>Sleep algorithms is used only within these primary bedtimes</t>
+  </si>
+  <si>
+    <t>Slepp algorithm is not used for extra bedtimes</t>
+  </si>
+  <si>
+    <t>Upright_1</t>
+  </si>
+  <si>
+    <t>Time of all upright activities/postures (i.e. Stand + Move + Walk + Run + Stair)</t>
+  </si>
+  <si>
     <t>References:
-Influence of Anthropometrics on Step-Rate Thresholds for Moderate and Vigorous Physical Activity in Older Adults: Scientific Modeling Study
-DOI: 10.2196/12363
-Tudor-Locke C, Han H, Aguiar EJ, et alHow fast is fast enough? Walking cadence (steps/min) as a practical estimate of intensity in adults: a narrative reviewBritish Journal of Sports Medicine 2018;52:776-788.
+Influence of Anthropometrics on Step-Rate Thresholds for Moderate and Vigorous Physical Activity in Older Adults: Scientific Modeling Study DOI: 10.2196/12363
+How fast is fast enough? Walking cadence (steps/min) as a practical estimate of intensity in adults: a narrative review http://dx.doi.org/10.1136/bjsports-2017-097628
 % activity to MET translation (these values are used to give each-epoch an equivalent 'MET' value. In other words we create a continuous variable with a resolution of 1s
 Settings.MET_SI=0.90;
 Settings.MET_LieStill=0.95;
@@ -989,90 +1063,12 @@
 Settings.MET_Cycle=7;
 Settings.MET_Other=2; % "Other" with no periodicity falls into light physical activity and given a fixed MET value of 2, "Other" with periodicity as classified similar to Walk.
 % Then above continuous variable is discretized back into the categorical intensity classes given below with given cutoffs
-Settings.PA_Slp=0.0;
-Settings.PA_SED=0.95;  % lieStill belongs to sedentary
-Settings.PA_LPA=1.5;
-Settings.PA_LPA_Amb=1.6; %introduce another called LPA_ambulatory to seperate standing from other LPA activities
-Settings.PA_MPA=3.0;
-Settings.PA_VPA=6.0;</t>
-  </si>
-  <si>
-    <t>Number of leisure days detected. A leisure day is where some or whole part of the day is flagged as leisure, but not as work. Not available for ProPASS tables.</t>
-  </si>
-  <si>
-    <t>Number of work days detected. A work day is a day where some time of the day is flagged as "Work" by  diary. Not available for ProPASS tables.</t>
-  </si>
-  <si>
-    <t>Day_QC_1</t>
-  </si>
-  <si>
-    <t>NotEnoughWear_1</t>
-  </si>
-  <si>
-    <t>NoWlk_1</t>
-  </si>
-  <si>
-    <t>TooMuchOther_1</t>
-  </si>
-  <si>
-    <t>TooMuchStair_1</t>
-  </si>
-  <si>
-    <t>NoSleepInt_1</t>
-  </si>
-  <si>
-    <t>NumPrimaryBDs_1</t>
-  </si>
-  <si>
-    <t>NumExtraBDs_1</t>
-  </si>
-  <si>
-    <t>The auto detected quality check flag for the day. ProPASS wide-format table contains days only days where this flag is "OK"</t>
-  </si>
-  <si>
-    <t>A flag indicating if the day has less than 30s of walking</t>
-  </si>
-  <si>
-    <t>When a day has not enough walking, it affects the individual calibration (refrence-positions) and it can then lead to less accurate classifications</t>
-  </si>
-  <si>
-    <t>A flag indicating if the day has not enough wear time (20 hrs). Should always be 0 under ProPASS mode</t>
-  </si>
-  <si>
-    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then it's a problem.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A flag indicating if more than 30 minutes of "other" exist in the day </t>
-  </si>
-  <si>
-    <t>A flag indicating more than 120 minutes of stair-walking present in the day.</t>
-  </si>
-  <si>
-    <t>Too much stair walking most probably means walking/hiking in steep hills,  confusion with bicycling (somewhat rare but possible) etc.</t>
-  </si>
-  <si>
-    <t>A sleep-interval (a mid-point of a sleep interval to be precise) is not found within the day</t>
-  </si>
-  <si>
-    <t>This is not necessarily a problem. If the missing sleep is a technical problem, this day will then have much higher sedentary times than the other days</t>
-  </si>
-  <si>
-    <t>Number of primary bedtimes (mid points) found within the current day</t>
-  </si>
-  <si>
-    <t>Number of possible extra bedtimes found within the current day</t>
-  </si>
-  <si>
-    <t>Sleep algorithms is used only within these primary bedtimes</t>
-  </si>
-  <si>
-    <t>Slepp algorithm is not used for extra bedtimes</t>
-  </si>
-  <si>
-    <t>Upright_1</t>
-  </si>
-  <si>
-    <t>Time of all upright activities/postures (i.e. Stand + Move + Walk + Run + Stair)</t>
+Settings.PA_Slp=0.0; % 
+Settings.PA_SED=0.95;  % cutoff for variable INT1 (lieStill belongs to sedentary)
+Settings.PA_LPA=1.5; % cutoff for variable INT2
+Settings.PA_LPA_Amb=1.6;  %  cutoff for variable INT2_Amb (introduce to seperate standing from other LPA activities)
+Settings.PA_MPA=3.0; % cutoff for variable  INT3 
+Settings.PA_VPA=6.0; %  cutoff for variable INT4</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1713,7 +1709,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="29" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1779,7 +1775,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>91</v>
@@ -1790,7 +1786,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>91</v>
@@ -1862,86 +1858,86 @@
     </row>
     <row r="19" spans="1:3" ht="30">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="30">
       <c r="A20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1996,7 +1992,7 @@
         <v>86</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C34" s="4"/>
     </row>
@@ -2005,7 +2001,7 @@
         <v>87</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="4"/>
     </row>
@@ -2029,7 +2025,7 @@
         <v>18</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C38" s="10"/>
     </row>
@@ -2038,7 +2034,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C39" s="10"/>
     </row>
@@ -2047,7 +2043,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C40" s="4"/>
     </row>
@@ -2062,10 +2058,10 @@
     </row>
     <row r="42" spans="1:3" ht="45">
       <c r="A42" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
@@ -2079,7 +2075,7 @@
         <v>27</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C44" s="4"/>
     </row>
@@ -2182,10 +2178,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C56" s="4"/>
     </row>
@@ -2207,9 +2203,6 @@
       <c r="B59" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="60" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
       <c r="A60" s="25" t="s">
@@ -2219,7 +2212,7 @@
         <v>46</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2263,7 +2256,7 @@
         <v>172</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2274,7 +2267,7 @@
         <v>177</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="5" customFormat="1">

</xml_diff>

<commit_message>
minor edits to variable definitions document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="18810"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="225">
   <si>
     <t>varNames</t>
   </si>
@@ -27,9 +27,6 @@
     <t>SubjectID</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
     <t>Batch</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
   </si>
   <si>
     <t>Number of days present in the accelerometer data after automatically trimming Non-wear (NW) days in the beginning and end</t>
-  </si>
-  <si>
-    <t>Following variables are derived daily. The suffix (in this case "_1") indicate the day number. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. Only days determined to be valid (see above) are listed in the table.</t>
   </si>
   <si>
     <t>Whether the  is a work-day or a leisure day. See definitions of number of work and leisure days above. Possible values "Work", "Leisure" or empty</t>
@@ -683,115 +677,6 @@
   </si>
   <si>
     <t xml:space="preserve">Time spent on different energy expenditure intensity classes </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The posture </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"SitLie"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
-    </r>
   </si>
   <si>
     <t>How times are derived</t>
@@ -1069,6 +954,127 @@
 Settings.PA_LPA_Amb=1.6;  %  cutoff for variable INT2_Amb (introduce to seperate standing from other LPA activities)
 Settings.PA_MPA=3.0; % cutoff for variable  INT3 
 Settings.PA_VPA=6.0; %  cutoff for variable INT4</t>
+  </si>
+  <si>
+    <t>Following variables are derived daily. The suffix (in this case "_1") indicate the day number. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. Only days determined to be valid (see below) are listed in the table.</t>
+  </si>
+  <si>
+    <t>QC_Status</t>
+  </si>
+  <si>
+    <t>possible values: "OK", "Check" or "NotOK"</t>
+  </si>
+  <si>
+    <t>Ex. 2022-03-28 15.12.34</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The posture </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"SitLie"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1162,14 +1168,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1178,6 +1176,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1319,7 +1325,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1361,14 +1367,8 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1"/>
@@ -1381,10 +1381,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1393,8 +1393,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1408,6 +1408,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1696,257 +1702,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="29" customFormat="1" ht="20.25" thickBot="1">
-      <c r="A1" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.399999999999999" thickBot="1">
+      <c r="A1" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30.75" thickTop="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.4" thickTop="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>220</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="30">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.8">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="30">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
-      <c r="A10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>196</v>
+      <c r="B10" s="29" t="s">
+        <v>192</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" s="18" customFormat="1" ht="60">
-      <c r="B12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="19"/>
+    <row r="12" spans="1:3" s="17" customFormat="1" ht="57.6">
+      <c r="B12" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" ht="28.8">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="30">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="30">
+    <row r="19" spans="1:3" ht="28.8">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="30">
+        <v>202</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8">
+      <c r="A22" t="s">
+        <v>197</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30">
-      <c r="A22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C22" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="14" customFormat="1" ht="90">
-      <c r="B28" s="17" t="s">
-        <v>128</v>
+    <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
+      <c r="B28" s="34" t="s">
+        <v>126</v>
       </c>
       <c r="C28" s="15"/>
     </row>
@@ -1955,748 +1967,748 @@
       <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B30" s="23" t="s">
-        <v>131</v>
+      <c r="B30" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="45">
+    <row r="34" spans="1:3" ht="43.2">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="45">
+    <row r="35" spans="1:3" ht="43.2">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
+      <c r="B37" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" ht="28.8">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B37" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" ht="30">
-      <c r="A38" t="s">
+      <c r="B38" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="86.4">
+      <c r="A39" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="90">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
       <c r="B39" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" ht="28.8">
+      <c r="A41" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" ht="30">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
       <c r="B41" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="45">
+    <row r="42" spans="1:3" ht="43.2">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B43" s="23" t="s">
-        <v>129</v>
+      <c r="B43" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" ht="30">
-      <c r="A46" t="s">
-        <v>29</v>
-      </c>
       <c r="B46" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" ht="43.2">
+      <c r="A48" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3" ht="45">
-      <c r="A48" t="s">
-        <v>39</v>
-      </c>
       <c r="B48" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="4"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:3" ht="30">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
       <c r="B54" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C56" s="4"/>
     </row>
     <row r="57" spans="1:3" ht="45.75" customHeight="1">
       <c r="A57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" s="5" customFormat="1">
+      <c r="C58" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="5" customFormat="1">
+      <c r="B59" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
+      <c r="A60" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" s="5" customFormat="1">
-      <c r="C58" s="22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="5" customFormat="1">
-      <c r="B59" s="22" t="s">
+      <c r="C60" s="24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="28.8">
+      <c r="A62" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="28.8">
+      <c r="A63" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="26" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
-      <c r="A60" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B60" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="30">
-      <c r="A62" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="B62" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C62" s="28" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="25" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="30">
-      <c r="A63" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="28" t="s">
+      <c r="B65" s="26" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="B64" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="27" t="s">
+      <c r="C65" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="5" customFormat="1">
+      <c r="A66" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B66" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="C65" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="5" customFormat="1">
-      <c r="A66" s="27" t="s">
+      <c r="C66" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="C66" s="28" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1">
-      <c r="A67" s="27"/>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1">
-      <c r="B68" s="21" t="s">
-        <v>90</v>
+      <c r="B68" s="19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="120">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="100.8">
       <c r="B74" s="12" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="C75" s="32" t="s">
-        <v>93</v>
+      <c r="C75" s="30" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="33"/>
+        <v>72</v>
+      </c>
+      <c r="C76" s="31"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C77" s="33"/>
+        <v>67</v>
+      </c>
+      <c r="C77" s="31"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" s="33"/>
+        <v>68</v>
+      </c>
+      <c r="C78" s="31"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C79" s="33"/>
+        <v>69</v>
+      </c>
+      <c r="C79" s="31"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="33"/>
+        <v>73</v>
+      </c>
+      <c r="C80" s="31"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C81" s="33"/>
+        <v>70</v>
+      </c>
+      <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" s="31"/>
+    </row>
+    <row r="83" spans="1:3" ht="28.8">
+      <c r="A83" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C82" s="33"/>
-    </row>
-    <row r="83" spans="1:3" ht="30">
-      <c r="A83" t="s">
-        <v>37</v>
-      </c>
       <c r="B83" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C83" s="33"/>
-    </row>
-    <row r="86" spans="1:3" s="5" customFormat="1" ht="75">
-      <c r="B86" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C86" s="24" t="s">
-        <v>94</v>
+        <v>78</v>
+      </c>
+      <c r="C83" s="31"/>
+    </row>
+    <row r="86" spans="1:3" s="5" customFormat="1" ht="72">
+      <c r="B86" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C88" s="34" t="s">
-        <v>127</v>
+        <v>93</v>
+      </c>
+      <c r="C88" s="32" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="34"/>
+        <v>94</v>
+      </c>
+      <c r="C89" s="32"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C90" s="34"/>
+        <v>95</v>
+      </c>
+      <c r="C90" s="32"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="C91" s="32"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C92" s="34"/>
+        <v>97</v>
+      </c>
+      <c r="C92" s="32"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C93" s="34"/>
+        <v>98</v>
+      </c>
+      <c r="C93" s="32"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" s="34"/>
+        <v>99</v>
+      </c>
+      <c r="C94" s="32"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C95" s="34"/>
+        <v>100</v>
+      </c>
+      <c r="C95" s="32"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C96" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="C96" s="32"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C97" s="34"/>
+        <v>102</v>
+      </c>
+      <c r="C97" s="32"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C98" s="34"/>
+        <v>103</v>
+      </c>
+      <c r="C98" s="32"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C99" s="34"/>
+        <v>104</v>
+      </c>
+      <c r="C99" s="32"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C100" s="34"/>
+        <v>105</v>
+      </c>
+      <c r="C100" s="32"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C101" s="34"/>
+        <v>106</v>
+      </c>
+      <c r="C101" s="32"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C102" s="34"/>
+        <v>107</v>
+      </c>
+      <c r="C102" s="32"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C103" s="34"/>
+        <v>108</v>
+      </c>
+      <c r="C103" s="32"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C104" s="34"/>
+        <v>109</v>
+      </c>
+      <c r="C104" s="32"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C105" s="34"/>
+        <v>110</v>
+      </c>
+      <c r="C105" s="32"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C106" s="34"/>
+        <v>111</v>
+      </c>
+      <c r="C106" s="32"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C107" s="34"/>
+        <v>112</v>
+      </c>
+      <c r="C107" s="32"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C108" s="34"/>
+        <v>113</v>
+      </c>
+      <c r="C108" s="32"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C109" s="34"/>
+        <v>114</v>
+      </c>
+      <c r="C109" s="32"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C110" s="34"/>
+        <v>115</v>
+      </c>
+      <c r="C110" s="32"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C111" s="34"/>
+        <v>116</v>
+      </c>
+      <c r="C111" s="32"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C112" s="34"/>
+        <v>124</v>
+      </c>
+      <c r="C112" s="32"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C113" s="34"/>
+        <v>117</v>
+      </c>
+      <c r="C113" s="32"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C114" s="34"/>
+        <v>118</v>
+      </c>
+      <c r="C114" s="32"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C115" s="34"/>
+        <v>119</v>
+      </c>
+      <c r="C115" s="32"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C116" s="34"/>
+        <v>120</v>
+      </c>
+      <c r="C116" s="32"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C117" s="34"/>
+        <v>121</v>
+      </c>
+      <c r="C117" s="32"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C118" s="34"/>
+        <v>122</v>
+      </c>
+      <c r="C118" s="32"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C119" s="34"/>
+        <v>123</v>
+      </c>
+      <c r="C119" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Improvements to Variable-definitions document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="18810"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -930,150 +930,209 @@
     <t>Time of all upright activities/postures (i.e. Stand + Move + Walk + Run + Stair)</t>
   </si>
   <si>
-    <t>References:
+    <t>Following variables are derived daily. The suffix (in this case "_1") indicate the day number. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. Only days determined to be valid (see below) are listed in the table.</t>
+  </si>
+  <si>
+    <t>QC_Status</t>
+  </si>
+  <si>
+    <t>possible values: "OK", "Check" or "NotOK"</t>
+  </si>
+  <si>
+    <t>Ex. 2022-03-28 15.12.34</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The posture </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"SitLie"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>References:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF833C0C"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 Influence of Anthropometrics on Step-Rate Thresholds for Moderate and Vigorous Physical Activity in Older Adults: Scientific Modeling Study DOI: 10.2196/12363
 How fast is fast enough? Walking cadence (steps/min) as a practical estimate of intensity in adults: a narrative review http://dx.doi.org/10.1136/bjsports-2017-097628
-% activity to MET translation (these values are used to give each-epoch an equivalent 'MET' value. In other words we create a continuous variable with a resolution of 1s
-Settings.MET_SI=0.90;
-Settings.MET_LieStill=0.95;
-Settings.MET_Lie=1.0;
-Settings.MET_Sit=1.3;
-Settings.MET_Stand=1.55;
-Settings.MET_Move=2.0;
-Settings.Wlk_Low_MET=2;
-Settings.Wlk_Fast_MET=4;
-Settings.Wlk_VFast_MET=7;
-Settings.MET_Running=10;
-Settings.MET_Stairs=8;
-Settings.MET_Cycle=7;
-Settings.MET_Other=2; % "Other" with no periodicity falls into light physical activity and given a fixed MET value of 2, "Other" with periodicity as classified similar to Walk.
-% Then above continuous variable is discretized back into the categorical intensity classes given below with given cutoffs
-Settings.PA_Slp=0.0; % 
-Settings.PA_SED=0.95;  % cutoff for variable INT1 (lieStill belongs to sedentary)
-Settings.PA_LPA=1.5; % cutoff for variable INT2
-Settings.PA_LPA_Amb=1.6;  %  cutoff for variable INT2_Amb (introduce to seperate standing from other LPA activities)
-Settings.PA_MPA=3.0; % cutoff for variable  INT3 
-Settings.PA_VPA=6.0; %  cutoff for variable INT4</t>
-  </si>
-  <si>
-    <t>Following variables are derived daily. The suffix (in this case "_1") indicate the day number. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. Only days determined to be valid (see below) are listed in the table.</t>
-  </si>
-  <si>
-    <t>QC_Status</t>
-  </si>
-  <si>
-    <t>possible values: "OK", "Check" or "NotOK"</t>
-  </si>
-  <si>
-    <t>Ex. 2022-03-28 15.12.34</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bouts related variables of  activity/posture/intensity-classes.   The combined posture "SitLie" is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Activity to MET translation (these values are used to give each-epoch an equivalent 'MET' value. In other words we create a continuous variable with a resolution of 1s</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF833C0C"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
+MET_SI = 0.90
+MET_LieStill = 0.95
+MET_Lie = 1.0
+MET_Sit = 1.3
+MET_Stand = 1.55
+MET_Move = 2.0
+MET_Walk_Low_ = 2 (&lt; 100 Steps/min)
+MET_Walk_Fast = 4 (&gt;= 100 Steps/min)
+MET_Walk_VeryFast = 7 (&gt;= 135 Steps/min)
+MET_Running = 10
+MET_Stairs = 8
+MET_Cycle = 7
+MET_Other = 2  ("Other" with no periodicity falls into light physical activity and given a fixed MET value of 2, "Other" with periodicity as classified similar to Walk)
 </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">The posture </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"SitLie"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Then above continuous variable is discretized back into the categorical intensity classes given below with given cutoffs</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF833C0C"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Upright, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
-</t>
+PA_Slp = 0.9
+PA_INT1 = 0.95 (cutoff for variable INT1; lieStill belongs to sedentary)
+PA_INT2 = 1.5 (cutoff for variable INT2)
+PA_INT2_Amb = 1.6  (cutoff for variable INT2_Amb - introduce to seperate standing from other LPA activities)
+PA_INT3 = 3.0 (cutoff for variable  INT3)
+PA_INT4 = 6.0 (cutoff for variable INT4)</t>
     </r>
   </si>
 </sst>
@@ -1081,7 +1140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1187,6 +1246,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1400,6 +1466,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1408,12 +1480,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1703,24 +1769,24 @@
   <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.109375" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.399999999999999" thickBot="1">
+    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>187</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1"/>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -1732,7 +1798,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29.4" thickTop="1">
+    <row r="4" spans="1:3" ht="30.75" thickTop="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1740,15 +1806,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1759,10 +1825,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1780,7 +1846,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.8">
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="30">
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1791,7 +1857,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -1806,9 +1872,9 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" s="17" customFormat="1" ht="57.6">
-      <c r="B12" s="33" t="s">
-        <v>219</v>
+    <row r="12" spans="1:3" s="17" customFormat="1" ht="60">
+      <c r="B12" s="30" t="s">
+        <v>218</v>
       </c>
       <c r="C12" s="18"/>
     </row>
@@ -1839,7 +1905,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="28.8">
+    <row r="16" spans="1:3" ht="30">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1866,7 +1932,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="28.8">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" t="s">
         <v>194</v>
       </c>
@@ -1874,10 +1940,10 @@
         <v>202</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28.8">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
       <c r="A20" t="s">
         <v>195</v>
       </c>
@@ -1897,7 +1963,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8">
+    <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
         <v>197</v>
       </c>
@@ -1919,7 +1985,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -1956,8 +2022,8 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
-      <c r="B28" s="34" t="s">
+    <row r="28" spans="1:3" s="14" customFormat="1" ht="90">
+      <c r="B28" s="31" t="s">
         <v>126</v>
       </c>
       <c r="C28" s="15"/>
@@ -1999,7 +2065,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="43.2">
+    <row r="34" spans="1:3" ht="45">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -2008,7 +2074,7 @@
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="43.2">
+    <row r="35" spans="1:3" ht="45">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -2032,7 +2098,7 @@
       </c>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" ht="28.8">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2041,7 +2107,7 @@
       </c>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="86.4">
+    <row r="39" spans="1:3" ht="90">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2059,7 +2125,7 @@
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="28.8">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2068,7 +2134,7 @@
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="43.2">
+    <row r="42" spans="1:3" ht="45">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -2100,7 +2166,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="30">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2118,7 +2184,7 @@
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="43.2">
+    <row r="48" spans="1:3" ht="45">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -2170,7 +2236,7 @@
       </c>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" ht="30">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2224,7 +2290,7 @@
         <v>45</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2238,7 +2304,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="28.8">
+    <row r="62" spans="1:3" ht="30">
       <c r="A62" s="25" t="s">
         <v>165</v>
       </c>
@@ -2249,7 +2315,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="28.8">
+    <row r="63" spans="1:3" ht="30">
       <c r="A63" s="25" t="s">
         <v>167</v>
       </c>
@@ -2327,16 +2393,16 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="100.8">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="120">
       <c r="B74" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="C75" s="30" t="s">
+      <c r="C75" s="32" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2347,7 +2413,7 @@
       <c r="B76" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="31"/>
+      <c r="C76" s="33"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
@@ -2356,7 +2422,7 @@
       <c r="B77" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="31"/>
+      <c r="C77" s="33"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
@@ -2365,7 +2431,7 @@
       <c r="B78" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C78" s="31"/>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
@@ -2374,7 +2440,7 @@
       <c r="B79" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="31"/>
+      <c r="C79" s="33"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
@@ -2383,7 +2449,7 @@
       <c r="B80" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="31"/>
+      <c r="C80" s="33"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -2392,7 +2458,7 @@
       <c r="B81" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C81" s="31"/>
+      <c r="C81" s="33"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -2401,20 +2467,20 @@
       <c r="B82" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C82" s="31"/>
-    </row>
-    <row r="83" spans="1:3" ht="28.8">
+      <c r="C82" s="33"/>
+    </row>
+    <row r="83" spans="1:3" ht="30">
       <c r="A83" t="s">
         <v>36</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C83" s="31"/>
-    </row>
-    <row r="86" spans="1:3" s="5" customFormat="1" ht="72">
+      <c r="C83" s="33"/>
+    </row>
+    <row r="86" spans="1:3" s="5" customFormat="1" ht="75">
       <c r="B86" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>92</v>
@@ -2427,7 +2493,7 @@
       <c r="B88" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="C88" s="34" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2438,7 +2504,7 @@
       <c r="B89" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C89" s="32"/>
+      <c r="C89" s="34"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
@@ -2447,7 +2513,7 @@
       <c r="B90" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C90" s="32"/>
+      <c r="C90" s="34"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
@@ -2456,7 +2522,7 @@
       <c r="B91" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C91" s="32"/>
+      <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
@@ -2465,7 +2531,7 @@
       <c r="B92" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C92" s="32"/>
+      <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
@@ -2474,7 +2540,7 @@
       <c r="B93" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C93" s="32"/>
+      <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
@@ -2483,7 +2549,7 @@
       <c r="B94" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C94" s="32"/>
+      <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
@@ -2492,7 +2558,7 @@
       <c r="B95" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C95" s="32"/>
+      <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
@@ -2501,7 +2567,7 @@
       <c r="B96" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C96" s="32"/>
+      <c r="C96" s="34"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
@@ -2510,7 +2576,7 @@
       <c r="B97" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="32"/>
+      <c r="C97" s="34"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
@@ -2519,7 +2585,7 @@
       <c r="B98" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C98" s="32"/>
+      <c r="C98" s="34"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
@@ -2528,7 +2594,7 @@
       <c r="B99" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C99" s="32"/>
+      <c r="C99" s="34"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
@@ -2537,7 +2603,7 @@
       <c r="B100" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C100" s="32"/>
+      <c r="C100" s="34"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
@@ -2546,7 +2612,7 @@
       <c r="B101" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C101" s="32"/>
+      <c r="C101" s="34"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
@@ -2555,7 +2621,7 @@
       <c r="B102" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C102" s="32"/>
+      <c r="C102" s="34"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
@@ -2564,7 +2630,7 @@
       <c r="B103" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C103" s="32"/>
+      <c r="C103" s="34"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
@@ -2573,7 +2639,7 @@
       <c r="B104" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C104" s="32"/>
+      <c r="C104" s="34"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
@@ -2582,7 +2648,7 @@
       <c r="B105" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C105" s="32"/>
+      <c r="C105" s="34"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
@@ -2591,7 +2657,7 @@
       <c r="B106" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C106" s="32"/>
+      <c r="C106" s="34"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
@@ -2600,7 +2666,7 @@
       <c r="B107" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C107" s="32"/>
+      <c r="C107" s="34"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
@@ -2609,7 +2675,7 @@
       <c r="B108" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C108" s="32"/>
+      <c r="C108" s="34"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
@@ -2618,7 +2684,7 @@
       <c r="B109" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C109" s="32"/>
+      <c r="C109" s="34"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
@@ -2627,7 +2693,7 @@
       <c r="B110" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C110" s="32"/>
+      <c r="C110" s="34"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
@@ -2636,7 +2702,7 @@
       <c r="B111" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C111" s="32"/>
+      <c r="C111" s="34"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
@@ -2645,7 +2711,7 @@
       <c r="B112" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C112" s="32"/>
+      <c r="C112" s="34"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
@@ -2654,7 +2720,7 @@
       <c r="B113" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C113" s="32"/>
+      <c r="C113" s="34"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
@@ -2663,7 +2729,7 @@
       <c r="B114" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C114" s="32"/>
+      <c r="C114" s="34"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
@@ -2672,7 +2738,7 @@
       <c r="B115" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C115" s="32"/>
+      <c r="C115" s="34"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
@@ -2681,7 +2747,7 @@
       <c r="B116" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C116" s="32"/>
+      <c r="C116" s="34"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
@@ -2690,7 +2756,7 @@
       <c r="B117" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C117" s="32"/>
+      <c r="C117" s="34"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
@@ -2699,7 +2765,7 @@
       <c r="B118" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C118" s="32"/>
+      <c r="C118" s="34"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
@@ -2708,7 +2774,7 @@
       <c r="B119" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C119" s="32"/>
+      <c r="C119" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Improvements to variable definitions
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
   <si>
     <t>varNames</t>
   </si>
@@ -246,15 +246,9 @@
     <t>The total times of sleep within a bedtime. This is also the time of sleep inside sleep_intervals by definition of sleep-interval.</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto detected preliminary quality check (QC) flag. QC flag is auto detected using predefined outlier criteria. Additionally technical errors can also generate QC flag. </t>
-  </si>
-  <si>
     <t>Number of days present in the accelerometer data after automatically trimming Non-wear (NW) days in the beginning and end</t>
   </si>
   <si>
-    <t>Whether the  is a work-day or a leisure day. See definitions of number of work and leisure days above. Possible values "Work", "Leisure" or empty</t>
-  </si>
-  <si>
     <t>Number of breaks of sitting or lying postures. (i.e. this is the number of times a person rises from a sitting or a lying posture)</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>Time of stair-walking (all stair walking like activities are counted. i.e. terrain walking etc.)</t>
   </si>
   <si>
-    <t>Time of activities in "Other" postures/activities which has somewhat horizontal thigh position. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
-  </si>
-  <si>
     <t>Number of steps during walking</t>
   </si>
   <si>
@@ -286,9 +277,6 @@
   </si>
   <si>
     <t>Cadence related variables. Cadence is only detected for walking, running and stair-walking</t>
-  </si>
-  <si>
-    <t>Only available when work/leisure diary is given</t>
   </si>
   <si>
     <t>Important Note: These variables are calculated using the direct output of activity detection algorithm with an epoch of 1s. Any sporadic break, misclassification or ambiguity can affect these variables. These variables, except for the combined activity/posture "SitLie", should only be used with consultation of ActiPASS developers</t>
@@ -691,9 +679,6 @@
     <t>LieStill_1</t>
   </si>
   <si>
-    <t>The total time of possible sleep outside a bedtime (this is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes.). In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
-  </si>
-  <si>
     <t>Time of lying. If LieStill is defined, time of 'Lie' also contains that time.</t>
   </si>
   <si>
@@ -704,124 +689,6 @@
   </si>
   <si>
     <r>
-      <t>The time of</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> NW outside any periods flagged as sleep-intervals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>. There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> not a part of Awake_1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>variable below</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>The time of</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> NW inside any periods flagged as sleep-intervals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>not a part of SleepInterval_1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> below</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The  time </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>within ValidDuration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> of this calendar day which is flagged as</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> belonging to a sleep-interval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.
- A sleep interval is theoretically defined as the time between the first sleep onset and the last awakening. Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>The time</t>
     </r>
     <r>
@@ -850,12 +717,6 @@
       </rPr>
       <t>not flagged as belonging to a sleep-interval</t>
     </r>
-  </si>
-  <si>
-    <t>Number of leisure days detected. A leisure day is where some or whole part of the day is flagged as leisure, but not as work. Not available for ProPASS tables.</t>
-  </si>
-  <si>
-    <t>Number of work days detected. A work day is a day where some time of the day is flagged as "Work" by  diary. Not available for ProPASS tables.</t>
   </si>
   <si>
     <t>Day_QC_1</t>
@@ -1134,6 +995,187 @@
 PA_INT3 = 3.0 (cutoff for variable  INT3)
 PA_INT4 = 6.0 (cutoff for variable INT4)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>The time of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> NW outside any periods flagged as sleep-intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> not a part of Awake_1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>variable below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The time of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> NW inside any periods flagged as sleep-intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not a part of SleepInterval_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> below</t>
+    </r>
+  </si>
+  <si>
+    <t>A sleep interval is theoretically defined as the time between the first sleep onset and the last awakening. Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The  time </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>within ValidDuration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of this calendar day which is flagged as</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> belonging to a sleep-interval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The total time of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>possible sleep outside a bedtime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> (this is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes.).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time of activities in "Other" postures/activities which has somewhat horizontal thigh position. </t>
+  </si>
+  <si>
+    <t>Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the  is a work-day or a leisure day. </t>
+  </si>
+  <si>
+    <t>See definitions of number of work and leisure days above. Possible values "Work", "Leisure" or empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto detected preliminary quality check (QC) flag. </t>
+  </si>
+  <si>
+    <t>QC flag is auto detected using predefined outlier criteria. Additionally technical errors can also generate QC flag. Possible values: "OK", "Check" or "NotOK"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of work days detected. A work day is a day where some time of the day is flagged as "Work" by  diary. </t>
+  </si>
+  <si>
+    <t>Not available for ProPASS tables. Only available when work/leisure diary is given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of leisure days detected. A leisure day is where some or whole part of the day is flagged as leisure, but not as work. </t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1435,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1463,9 +1505,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1481,6 +1520,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -1768,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75:C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1781,7 +1824,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="27" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="27" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1795,7 +1838,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29.4" thickTop="1">
@@ -1806,15 +1849,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>75</v>
+        <v>209</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1825,7 +1868,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8">
@@ -1833,7 +1876,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -1850,22 +1893,22 @@
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>89</v>
+      <c r="B9" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>89</v>
+      <c r="B10" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1873,8 +1916,8 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" s="17" customFormat="1" ht="57.6">
-      <c r="B12" s="30" t="s">
-        <v>218</v>
+      <c r="B12" s="29" t="s">
+        <v>208</v>
       </c>
       <c r="C12" s="18"/>
     </row>
@@ -1905,14 +1948,16 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="28.8">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="4"/>
+      <c r="B16" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
@@ -1934,88 +1979,88 @@
     </row>
     <row r="19" spans="1:3" ht="28.8">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8">
       <c r="A20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>195</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>205</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.8">
       <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="C22" s="10" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>208</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2023,8 +2068,8 @@
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
-      <c r="B28" s="31" t="s">
-        <v>126</v>
+      <c r="B28" s="30" t="s">
+        <v>122</v>
       </c>
       <c r="C28" s="15"/>
     </row>
@@ -2034,7 +2079,7 @@
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
       <c r="B30" s="21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -2061,40 +2106,44 @@
         <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="43.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" ht="43.2">
+        <v>215</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C35" s="4"/>
+        <v>217</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
       <c r="B37" s="21" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C37" s="6"/>
     </row>
@@ -2103,25 +2152,27 @@
         <v>17</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="86.4">
+    <row r="39" spans="1:3" ht="28.8">
       <c r="A39" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="C39" s="10"/>
+        <v>220</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C40" s="4"/>
     </row>
@@ -2129,22 +2180,25 @@
       <c r="A41" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="10" t="s">
         <v>74</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="43.2">
+    <row r="42" spans="1:3" ht="28.8">
       <c r="A42" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
       <c r="B43" s="21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C43" s="6"/>
     </row>
@@ -2153,7 +2207,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C44" s="4"/>
     </row>
@@ -2189,7 +2243,7 @@
         <v>38</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" s="4"/>
     </row>
@@ -2241,7 +2295,7 @@
         <v>42</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C54" s="4"/>
     </row>
@@ -2256,107 +2310,109 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3" ht="45.75" customHeight="1">
+    <row r="57" spans="1:3" ht="19.8" customHeight="1">
       <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="4"/>
+      <c r="B57" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1">
       <c r="C58" s="20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1">
       <c r="B59" s="20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
       <c r="A60" s="23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>45</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="28.8">
       <c r="A62" s="25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.8">
       <c r="A63" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="5" customFormat="1">
       <c r="A66" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1">
@@ -2366,7 +2422,7 @@
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1">
       <c r="B68" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2382,7 +2438,7 @@
         <v>24</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2395,15 +2451,15 @@
     </row>
     <row r="74" spans="1:3" s="5" customFormat="1" ht="100.8">
       <c r="B74" s="12" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="C75" s="32" t="s">
-        <v>91</v>
+      <c r="C75" s="31" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2413,7 +2469,7 @@
       <c r="B76" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="33"/>
+      <c r="C76" s="32"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
@@ -2422,7 +2478,7 @@
       <c r="B77" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="33"/>
+      <c r="C77" s="32"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
@@ -2431,7 +2487,7 @@
       <c r="B78" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C78" s="33"/>
+      <c r="C78" s="32"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
@@ -2440,7 +2496,7 @@
       <c r="B79" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="33"/>
+      <c r="C79" s="32"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
@@ -2449,7 +2505,7 @@
       <c r="B80" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="33"/>
+      <c r="C80" s="32"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -2458,7 +2514,7 @@
       <c r="B81" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C81" s="33"/>
+      <c r="C81" s="32"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -2467,314 +2523,314 @@
       <c r="B82" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C82" s="33"/>
+      <c r="C82" s="32"/>
     </row>
     <row r="83" spans="1:3" ht="28.8">
       <c r="A83" t="s">
         <v>36</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C83" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C83" s="32"/>
     </row>
     <row r="86" spans="1:3" s="5" customFormat="1" ht="72">
       <c r="B86" s="21" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C88" s="34" t="s">
-        <v>125</v>
+        <v>89</v>
+      </c>
+      <c r="C88" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C89" s="34"/>
+        <v>90</v>
+      </c>
+      <c r="C89" s="33"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" s="34"/>
+        <v>91</v>
+      </c>
+      <c r="C90" s="33"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C91" s="34"/>
+        <v>92</v>
+      </c>
+      <c r="C91" s="33"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C92" s="34"/>
+        <v>93</v>
+      </c>
+      <c r="C92" s="33"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C93" s="34"/>
+        <v>94</v>
+      </c>
+      <c r="C93" s="33"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C94" s="34"/>
+        <v>95</v>
+      </c>
+      <c r="C94" s="33"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C95" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="C95" s="33"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C96" s="34"/>
+        <v>97</v>
+      </c>
+      <c r="C96" s="33"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C97" s="34"/>
+        <v>98</v>
+      </c>
+      <c r="C97" s="33"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C98" s="34"/>
+        <v>99</v>
+      </c>
+      <c r="C98" s="33"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C99" s="34"/>
+        <v>100</v>
+      </c>
+      <c r="C99" s="33"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C100" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="C100" s="33"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C101" s="34"/>
+        <v>102</v>
+      </c>
+      <c r="C101" s="33"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C102" s="34"/>
+        <v>103</v>
+      </c>
+      <c r="C102" s="33"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C103" s="34"/>
+        <v>104</v>
+      </c>
+      <c r="C103" s="33"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C104" s="34"/>
+        <v>105</v>
+      </c>
+      <c r="C104" s="33"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C105" s="34"/>
+        <v>106</v>
+      </c>
+      <c r="C105" s="33"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C106" s="34"/>
+        <v>107</v>
+      </c>
+      <c r="C106" s="33"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C107" s="34"/>
+        <v>108</v>
+      </c>
+      <c r="C107" s="33"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C108" s="34"/>
+        <v>109</v>
+      </c>
+      <c r="C108" s="33"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C109" s="34"/>
+        <v>110</v>
+      </c>
+      <c r="C109" s="33"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C110" s="34"/>
+        <v>111</v>
+      </c>
+      <c r="C110" s="33"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C111" s="34"/>
+        <v>112</v>
+      </c>
+      <c r="C111" s="33"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C112" s="34"/>
+        <v>120</v>
+      </c>
+      <c r="C112" s="33"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C113" s="34"/>
+        <v>113</v>
+      </c>
+      <c r="C113" s="33"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C114" s="34"/>
+        <v>114</v>
+      </c>
+      <c r="C114" s="33"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C115" s="34"/>
+        <v>115</v>
+      </c>
+      <c r="C115" s="33"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C116" s="34"/>
+        <v>116</v>
+      </c>
+      <c r="C116" s="33"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C117" s="34"/>
+        <v>117</v>
+      </c>
+      <c r="C117" s="33"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C118" s="34"/>
+        <v>118</v>
+      </c>
+      <c r="C118" s="33"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C119" s="34"/>
+        <v>119</v>
+      </c>
+      <c r="C119" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
variable definitions doc edits
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="18810"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -1812,24 +1812,25 @@
   <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>182</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="2" spans="1:3" ht="15" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -1841,7 +1842,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.75" thickTop="1">
+    <row r="4" spans="1:3" ht="29.4" thickTop="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1889,7 +1890,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="9" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1900,7 +1901,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="10" spans="1:3" s="11" customFormat="1" ht="28.8">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1916,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" s="17" customFormat="1" ht="60">
+    <row r="12" spans="1:3" s="17" customFormat="1" ht="57.6">
       <c r="B12" s="29" t="s">
         <v>208</v>
       </c>
@@ -1977,7 +1978,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="30">
+    <row r="19" spans="1:3" ht="28.8">
       <c r="A19" t="s">
         <v>184</v>
       </c>
@@ -1988,7 +1989,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
+    <row r="20" spans="1:3" ht="28.8">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -2008,7 +2009,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="28.8">
       <c r="A22" t="s">
         <v>187</v>
       </c>
@@ -2030,7 +2031,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -2067,7 +2068,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="14" customFormat="1" ht="90">
+    <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
       <c r="B28" s="30" t="s">
         <v>122</v>
       </c>
@@ -2147,7 +2148,7 @@
       </c>
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="28.8">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2156,7 +2157,7 @@
       </c>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="28.8">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2177,7 @@
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="28.8">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2185,7 +2186,7 @@
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="30">
+    <row r="42" spans="1:3" ht="28.8">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -2220,7 +2221,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="30">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>28</v>
       </c>
@@ -2238,7 +2239,7 @@
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="45">
+    <row r="48" spans="1:3" ht="43.2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -2290,7 +2291,7 @@
       </c>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:3" ht="30">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30">
+    <row r="62" spans="1:3" ht="28.8">
       <c r="A62" s="25" t="s">
         <v>161</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="30">
+    <row r="63" spans="1:3" ht="28.8">
       <c r="A63" s="25" t="s">
         <v>163</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="120">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="100.8">
       <c r="B74" s="12" t="s">
         <v>213</v>
       </c>
@@ -2525,7 +2526,7 @@
       </c>
       <c r="C82" s="34"/>
     </row>
-    <row r="83" spans="1:3" ht="30">
+    <row r="83" spans="1:3" ht="28.8">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -2534,7 +2535,7 @@
       </c>
       <c r="C83" s="34"/>
     </row>
-    <row r="86" spans="1:3" s="5" customFormat="1" ht="75">
+    <row r="86" spans="1:3" s="5" customFormat="1" ht="72">
       <c r="B86" s="21" t="s">
         <v>212</v>
       </c>

</xml_diff>

<commit_message>
Updated variable definition document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C8C3AD-F954-482D-A60A-6539652EF202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9AB0AB-830B-496B-B6E8-DEEFDED01F05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="233">
   <si>
     <t>varNames</t>
   </si>
@@ -1176,16 +1176,102 @@
     <t>Time spent on activities classified as moderate and vigorous  physical activity</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Following variables are derived daily. In the ProPASS wide-format table each variable is suffixed with day number. For example the suffix  "_1" in "Date_1" indicates the day number 1. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. Only days determined to be valid (see below) are listed in the table.
-</t>
+    <t xml:space="preserve">Following variables are derived daily. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>These variablesare saved to two different tables named "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ActiPASS_Daily_LongFormat_MasterFile.csv" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"ProPASS_WideFormat_MasterFile.csv"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+ In "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ProPASS_WideFormat_MasterFile.csv"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Only days determined to be valid (see below) are listed in the table.
+    Each variable is suffixed with day number. For example the suffix  "_1" in "Date_1" indicates the day number 1. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1298,6 +1384,28 @@
       <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1438,7 +1546,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1479,9 +1587,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1518,6 +1623,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1812,26 +1927,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C118"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="31.109375" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="27" customFormat="1" ht="20.399999999999999" thickBot="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:3" s="26" customFormat="1" ht="20.399999999999999" thickBot="1">
+      <c r="A1" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1"/>
     <row r="3" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
@@ -1897,10 +2012,10 @@
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1908,934 +2023,940 @@
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="17" customFormat="1" ht="81" customHeight="1">
-      <c r="B11" s="29" t="s">
+    <row r="11" spans="1:3" s="17" customFormat="1" ht="71.400000000000006" customHeight="1">
+      <c r="B11" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="18"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4"/>
+      <c r="C11" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>130</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>140</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="28.8">
-      <c r="A18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>115</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="28.8">
       <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8">
+      <c r="A20" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" ht="28.8">
+      <c r="A22" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>150</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" s="14" customFormat="1" ht="86.4">
-      <c r="B27" s="30" t="s">
+    <row r="27" spans="1:3">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" s="14" customFormat="1" ht="86.4">
+      <c r="B28" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="15"/>
-    </row>
-    <row r="28" spans="1:3" s="14" customFormat="1">
-      <c r="B28" s="16"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B29" s="21" t="s">
+    <row r="29" spans="1:3" s="14" customFormat="1">
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
+      <c r="B30" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>136</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B36" s="21" t="s">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
+      <c r="B37" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" ht="28.8">
-      <c r="A37" t="s">
-        <v>157</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" ht="28.8">
       <c r="A38" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="1:3" ht="28.8">
+      <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" ht="28.8">
-      <c r="A40" t="s">
-        <v>160</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" ht="28.8">
       <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" ht="28.8">
+      <c r="A42" t="s">
         <v>161</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B42" s="21" t="s">
+    <row r="43" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
+      <c r="B43" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>162</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>22</v>
+        <v>162</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>165</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" ht="43.2">
-      <c r="A47" t="s">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" ht="43.2">
+      <c r="A48" t="s">
         <v>166</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C49" s="4"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>169</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>171</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="4"/>
+        <v>170</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C53" s="4"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>174</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B56" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:3" ht="33" customHeight="1">
-      <c r="A56" t="s">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" ht="33" customHeight="1">
+      <c r="A57" t="s">
         <v>175</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B57" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1">
-      <c r="C57" s="20" t="s">
+    <row r="58" spans="1:3" s="5" customFormat="1">
+      <c r="C58" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1">
-      <c r="B58" s="20" t="s">
+    <row r="59" spans="1:3" s="5" customFormat="1">
+      <c r="B59" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
-      <c r="A59" s="23" t="s">
+    <row r="60" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
+      <c r="A60" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B60" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C60" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="25" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B61" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C61" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="28.8">
-      <c r="A61" s="25" t="s">
+    <row r="62" spans="1:3" ht="28.8">
+      <c r="A62" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B62" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C62" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="25" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B63" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C63" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="25" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="B64" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C64" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="25" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="B64" s="26" t="s">
+      <c r="B65" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="C65" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1">
-      <c r="A65" s="25" t="s">
+    <row r="66" spans="1:3" s="5" customFormat="1">
+      <c r="A66" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B66" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C66" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1">
-      <c r="A66" s="25"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
-    </row>
     <row r="67" spans="1:3" s="5" customFormat="1">
-      <c r="B67" s="19" t="s">
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+    </row>
+    <row r="68" spans="1:3" s="5" customFormat="1">
+      <c r="B68" s="18" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>184</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>182</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="100.8">
-      <c r="B73" s="12" t="s">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="100.8">
+      <c r="B74" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C74" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="C74" s="33" t="s">
+    <row r="75" spans="1:3">
+      <c r="C75" s="36" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>185</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="34"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" s="34"/>
+        <v>34</v>
+      </c>
+      <c r="C76" s="37"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="34"/>
+        <v>29</v>
+      </c>
+      <c r="C77" s="37"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="C78" s="37"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>189</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="34"/>
+        <v>188</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" s="37"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" s="34"/>
+        <v>35</v>
+      </c>
+      <c r="C80" s="37"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>190</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="37"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>191</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B82" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C81" s="34"/>
-    </row>
-    <row r="82" spans="1:3" ht="28.8">
-      <c r="A82" t="s">
+      <c r="C82" s="37"/>
+    </row>
+    <row r="83" spans="1:3" ht="28.8">
+      <c r="A83" t="s">
         <v>192</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C82" s="34"/>
-    </row>
-    <row r="85" spans="1:3" s="5" customFormat="1" ht="72">
-      <c r="B85" s="21" t="s">
+      <c r="C83" s="37"/>
+    </row>
+    <row r="86" spans="1:3" s="5" customFormat="1" ht="72">
+      <c r="B86" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C85" s="22" t="s">
+      <c r="C86" s="21" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>193</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C87" s="35" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C88" s="35"/>
+        <v>49</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C89" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="C89" s="38"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C90" s="35"/>
+        <v>51</v>
+      </c>
+      <c r="C90" s="38"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C91" s="35"/>
+        <v>52</v>
+      </c>
+      <c r="C91" s="38"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C92" s="35"/>
+        <v>53</v>
+      </c>
+      <c r="C92" s="38"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C93" s="35"/>
+        <v>54</v>
+      </c>
+      <c r="C93" s="38"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C94" s="35"/>
+        <v>55</v>
+      </c>
+      <c r="C94" s="38"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>209</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C95" s="35"/>
+        <v>208</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="38"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C96" s="35"/>
+        <v>57</v>
+      </c>
+      <c r="C96" s="38"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C97" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="C97" s="38"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C98" s="35"/>
+        <v>59</v>
+      </c>
+      <c r="C98" s="38"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C99" s="35"/>
+        <v>60</v>
+      </c>
+      <c r="C99" s="38"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C100" s="35"/>
+        <v>61</v>
+      </c>
+      <c r="C100" s="38"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C101" s="35"/>
+        <v>62</v>
+      </c>
+      <c r="C101" s="38"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C102" s="35"/>
+        <v>63</v>
+      </c>
+      <c r="C102" s="38"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>217</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="35"/>
+        <v>216</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C103" s="38"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C104" s="35"/>
+        <v>65</v>
+      </c>
+      <c r="C104" s="38"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C105" s="35"/>
+        <v>66</v>
+      </c>
+      <c r="C105" s="38"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C106" s="35"/>
+        <v>67</v>
+      </c>
+      <c r="C106" s="38"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C107" s="35"/>
+        <v>68</v>
+      </c>
+      <c r="C107" s="38"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C108" s="35"/>
+        <v>69</v>
+      </c>
+      <c r="C108" s="38"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C109" s="35"/>
+        <v>70</v>
+      </c>
+      <c r="C109" s="38"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C110" s="35"/>
+        <v>71</v>
+      </c>
+      <c r="C110" s="38"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>203</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C111" s="35"/>
+        <v>224</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111" s="38"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C112" s="35"/>
+        <v>80</v>
+      </c>
+      <c r="C112" s="38"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C113" s="35"/>
+        <v>73</v>
+      </c>
+      <c r="C113" s="38"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C114" s="35"/>
+        <v>74</v>
+      </c>
+      <c r="C114" s="38"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C115" s="35"/>
+        <v>75</v>
+      </c>
+      <c r="C115" s="38"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C116" s="35"/>
+        <v>76</v>
+      </c>
+      <c r="C116" s="38"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C117" s="35"/>
+        <v>77</v>
+      </c>
+      <c r="C117" s="38"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>197</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C118" s="38"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
         <v>196</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C118" s="35"/>
+      <c r="C119" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C74:C82"/>
-    <mergeCell ref="C87:C118"/>
+    <mergeCell ref="C75:C83"/>
+    <mergeCell ref="C88:C119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
minor edits to variable definition doc
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C757F-82A9-4FC1-AFE0-5C91EE3F12D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACB7066-6590-465A-9EA2-A96A3FAA190D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="18810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,28 +742,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>not a part of SleepInterval_1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> below</t>
-    </r>
-  </si>
-  <si>
     <t>A sleep interval is theoretically defined as the time between the first sleep onset and the last awakening. Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval</t>
   </si>
   <si>
@@ -830,9 +808,6 @@
     <t xml:space="preserve"> In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
   </si>
   <si>
-    <t xml:space="preserve">Time of activities in "Other" postures/activities which has somewhat horizontal thigh position. </t>
-  </si>
-  <si>
     <t>Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
   </si>
   <si>
@@ -855,28 +830,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of leisure days detected. A leisure day is where some or whole part of the day is flagged as leisure, but not as work. </t>
-  </si>
-  <si>
-    <r>
-      <t>There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> not a part of Awake_1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>variable below</t>
-    </r>
   </si>
   <si>
     <t>Date</t>
@@ -1301,6 +1254,53 @@
       </rPr>
       <t>) contains days only days where this flag is "OK"</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> not a part of Awake </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>variable below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not a part of SleepInterval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> below</t>
+    </r>
+  </si>
+  <si>
+    <t>Time of activities in "Other" postures/activities with movements which cannot be classified into known activities/postures</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1983,7 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="A3" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -2037,10 +2037,10 @@
         <v>111</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2051,7 +2051,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -2077,10 +2077,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
@@ -2088,18 +2088,18 @@
         <v>6</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
       <c r="B13" s="28" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
@@ -2108,7 +2108,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
@@ -2135,18 +2135,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>15</v>
@@ -2164,29 +2164,29 @@
     </row>
     <row r="21" spans="1:3" ht="30">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>98</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>101</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>102</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>104</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>106</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>107</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
       <c r="B30" s="29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C30" s="15"/>
     </row>
@@ -2272,7 +2272,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>16</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>17</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>43</v>
@@ -2299,29 +2299,29 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>115</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>116</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>117</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>42</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>97</v>
@@ -2345,18 +2345,18 @@
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>95</v>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="43" spans="1:3" ht="30">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>36</v>
@@ -2374,13 +2374,13 @@
     </row>
     <row r="44" spans="1:3" ht="30">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B44" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
@@ -2391,7 +2391,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>94</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>22</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="48" spans="1:3" ht="30">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>28</v>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>23</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="50" spans="1:3" ht="45">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>39</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>25</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>18</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>19</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>26</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="56" spans="1:3" ht="30">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>40</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>27</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>110</v>
@@ -2506,13 +2506,13 @@
     </row>
     <row r="59" spans="1:3" ht="33" customHeight="1">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="5" customFormat="1">
@@ -2538,10 +2538,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>86</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="64" spans="1:3" ht="30">
       <c r="A64" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>87</v>
@@ -2560,10 +2560,10 @@
     </row>
     <row r="65" spans="1:3" ht="30">
       <c r="A65" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>88</v>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>92</v>
@@ -2582,10 +2582,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>93</v>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1">
       <c r="A68" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>89</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>20</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>41</v>
@@ -2630,7 +2630,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>21</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>34</v>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>29</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>30</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>31</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>35</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>32</v>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>33</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="85" spans="1:3" ht="30">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>38</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>49</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>50</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>51</v>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>52</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>53</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>54</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>55</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>56</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>57</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>58</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>59</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>60</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>61</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>62</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>63</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>64</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B106" s="10" t="s">
         <v>65</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>66</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>67</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B109" s="10" t="s">
         <v>68</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B110" s="10" t="s">
         <v>69</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>70</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>71</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>72</v>
@@ -2949,7 +2949,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>80</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>73</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>74</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>75</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>76</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>77</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>78</v>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
variable definitions focus cell fix
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pashe866/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A52F3-0213-45ED-8708-3B90A9C04566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D9BC8A-7E55-594A-BA87-8900EE9DA1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="18810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30940" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -1310,7 +1310,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1986,37 +1986,37 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="26" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:3" s="26" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
     </row>
-    <row r="2" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
+    <row r="2" spans="1:3" s="26" customFormat="1" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
     </row>
-    <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" s="26" customFormat="1" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
         <v>227</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickTop="1"/>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
+    <row r="4" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30.75" thickTop="1">
+    <row r="6" spans="1:3" ht="33" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="11" spans="1:3" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="12" spans="1:3" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
+    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>223</v>
       </c>
@@ -2105,11 +2105,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
+    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>137</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>138</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>142</v>
       </c>
@@ -2253,27 +2253,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
+    <row r="30" spans="1:3" s="14" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="B30" s="29" t="s">
         <v>225</v>
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" s="14" customFormat="1">
+    <row r="31" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="16"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
+    <row r="32" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="20" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -2331,13 +2331,13 @@
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
+    <row r="39" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="20" t="s">
         <v>83</v>
       </c>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30">
+    <row r="44" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -2388,13 +2388,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
+    <row r="45" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="20" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>154</v>
       </c>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="30">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:3" ht="45">
+    <row r="50" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>160</v>
       </c>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>161</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>162</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="30">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>164</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>165</v>
       </c>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>166</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1">
+    <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -2520,17 +2520,17 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1">
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="C60" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
+    <row r="62" spans="1:3" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>85</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="24" t="s">
         <v>168</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="30">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="24" t="s">
         <v>169</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="24" t="s">
         <v>170</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
         <v>171</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
         <v>173</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1">
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>172</v>
       </c>
@@ -2607,17 +2607,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1">
+    <row r="69" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24"/>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1">
+    <row r="70" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>176</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>175</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>174</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="120">
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="B76" s="12" t="s">
         <v>113</v>
       </c>
@@ -2649,12 +2649,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77" s="37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="C78" s="38"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>178</v>
       </c>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="C79" s="38"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="C80" s="38"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>180</v>
       </c>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="C81" s="38"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>181</v>
       </c>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="C82" s="38"/>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>182</v>
       </c>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="C83" s="38"/>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>183</v>
       </c>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="C84" s="38"/>
     </row>
-    <row r="85" spans="1:3" ht="30">
+    <row r="85" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>184</v>
       </c>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="C85" s="38"/>
     </row>
-    <row r="88" spans="1:3" s="5" customFormat="1" ht="75">
+    <row r="88" spans="1:3" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="B88" s="20" t="s">
         <v>112</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>185</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>186</v>
       </c>
@@ -2754,7 +2754,7 @@
       </c>
       <c r="C91" s="39"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="C92" s="39"/>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>196</v>
       </c>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="C93" s="39"/>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>197</v>
       </c>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="C94" s="39"/>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>198</v>
       </c>
@@ -2790,7 +2790,7 @@
       </c>
       <c r="C95" s="39"/>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>199</v>
       </c>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="C96" s="39"/>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>200</v>
       </c>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="C97" s="39"/>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>201</v>
       </c>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="C98" s="39"/>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>202</v>
       </c>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="C99" s="39"/>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>203</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="C100" s="39"/>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="C101" s="39"/>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>205</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="C102" s="39"/>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>206</v>
       </c>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="C103" s="39"/>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="C104" s="39"/>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>208</v>
       </c>
@@ -2880,7 +2880,7 @@
       </c>
       <c r="C105" s="39"/>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="C106" s="39"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="C107" s="39"/>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>211</v>
       </c>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="C108" s="39"/>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>212</v>
       </c>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C109" s="39"/>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>213</v>
       </c>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="C110" s="39"/>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>214</v>
       </c>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="C111" s="39"/>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>215</v>
       </c>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="C112" s="39"/>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>216</v>
       </c>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="C113" s="39"/>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>195</v>
       </c>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="C114" s="39"/>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>194</v>
       </c>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="C115" s="39"/>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>193</v>
       </c>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="C116" s="39"/>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>192</v>
       </c>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="C117" s="39"/>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>191</v>
       </c>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C118" s="39"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>190</v>
       </c>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C119" s="39"/>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>189</v>
       </c>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="C120" s="39"/>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>188</v>
       </c>

</xml_diff>

<commit_message>
Added the missing "Bedtime" variable definition
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pashe866/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D9BC8A-7E55-594A-BA87-8900EE9DA1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338638C6-6601-4941-A248-351FA7F32967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30940" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="239">
   <si>
     <t>varNames</t>
   </si>
@@ -1303,14 +1303,23 @@
     <t>Time of activities in "Other" postures/activities with movements which cannot be classified into known activities/postures</t>
   </si>
   <si>
-    <t>This is same as "Sleep" now. Possible sleep outside bedtimes are now named "LieStill"</t>
+    <t>Bedtime</t>
+  </si>
+  <si>
+    <t>The time within this calendar day which is flagged as belonging to a bedtime</t>
+  </si>
+  <si>
+    <t>This is same as "Sleep" now since ActiPASS version 1.50. Possible sleep outside bedtimes are now named "LieStill"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A calendar day usually contains more than one (full or partial) bedtimes. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a bedtime. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1983,40 +1992,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="154.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="26" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="26" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
     </row>
-    <row r="2" spans="1:3" s="26" customFormat="1" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
     </row>
-    <row r="3" spans="1:3" s="26" customFormat="1" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="A3" s="36" t="s">
         <v>227</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" thickTop="1"/>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2036,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="33" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30.75" thickTop="1">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2057,7 +2066,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2066,7 +2075,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2084,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="11" customFormat="1" ht="30">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
       <c r="B13" s="28" t="s">
         <v>223</v>
       </c>
@@ -2105,11 +2114,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -2118,7 +2127,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -2127,7 +2136,7 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -2136,7 +2145,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -2156,7 +2165,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -2165,7 +2174,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -2176,7 +2185,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>137</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
         <v>138</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>142</v>
       </c>
@@ -2253,27 +2262,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" s="14" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
       <c r="B30" s="29" t="s">
         <v>225</v>
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="14" customFormat="1">
       <c r="B31" s="16"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
       <c r="B32" s="20" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="6"/>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -2282,7 +2291,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -2291,7 +2300,7 @@
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -2300,7 +2309,7 @@
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -2331,13 +2340,13 @@
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
       <c r="B39" s="20" t="s">
         <v>83</v>
       </c>
       <c r="C39" s="6"/>
     </row>
-    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -2346,688 +2355,699 @@
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30">
+      <c r="A42" t="s">
         <v>150</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B43" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" ht="30">
+      <c r="A44" t="s">
         <v>152</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C44" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30">
+      <c r="A45" t="s">
         <v>153</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B45" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="20" t="s">
+    <row r="46" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
+      <c r="B46" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B47" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="30">
+      <c r="A49" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:3" ht="45">
+      <c r="A51" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>162</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" ht="30">
+      <c r="A57" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B59" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" ht="33" customHeight="1">
+      <c r="A60" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B60" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C60" s="19" t="s">
+    <row r="61" spans="1:3" s="5" customFormat="1">
+      <c r="C61" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B61" s="19" t="s">
+    <row r="62" spans="1:3" s="5" customFormat="1">
+      <c r="B62" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+    <row r="63" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
+      <c r="A63" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B63" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C63" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="24" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B64" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="C63" s="25" t="s">
+      <c r="C64" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="24" t="s">
+    <row r="65" spans="1:3" ht="30">
+      <c r="A65" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B65" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C65" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
+    <row r="66" spans="1:3" ht="30">
+      <c r="A66" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B66" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C66" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="24" t="s">
+    <row r="67" spans="1:3">
+      <c r="A67" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B67" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="C67" s="25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="24" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B68" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C68" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="24" t="s">
+    <row r="69" spans="1:3" s="5" customFormat="1">
+      <c r="A69" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B69" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C69" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="24"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-    </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="18" t="s">
+    <row r="70" spans="1:3" s="5" customFormat="1">
+      <c r="A70" s="24"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+    </row>
+    <row r="71" spans="1:3" s="5" customFormat="1">
+      <c r="B71" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
         <v>176</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>175</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
         <v>174</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="B76" s="12" t="s">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="120">
+      <c r="B77" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C77" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C77" s="37" t="s">
+    <row r="78" spans="1:3">
+      <c r="C78" s="37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>177</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C78" s="38"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="C79" s="38"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>178</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C79" s="38"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="C80" s="38"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B81" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C80" s="38"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="C81" s="38"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>180</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C81" s="38"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="C82" s="38"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>181</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B83" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C82" s="38"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="C83" s="38"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
         <v>182</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B84" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C83" s="38"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="C84" s="38"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
         <v>183</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C84" s="38"/>
-    </row>
-    <row r="85" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="C85" s="38"/>
+    </row>
+    <row r="86" spans="1:3" ht="30">
+      <c r="A86" t="s">
         <v>184</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="38"/>
-    </row>
-    <row r="88" spans="1:3" s="5" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="B88" s="20" t="s">
+      <c r="C86" s="38"/>
+    </row>
+    <row r="89" spans="1:3" s="5" customFormat="1" ht="75">
+      <c r="B89" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C88" s="21" t="s">
+      <c r="C89" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>185</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B91" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="39" t="s">
+      <c r="C91" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>186</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B92" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C91" s="39"/>
-    </row>
-    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="C92" s="39"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>187</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B93" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C92" s="39"/>
-    </row>
-    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="C93" s="39"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>196</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B94" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="39"/>
-    </row>
-    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="C94" s="39"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
         <v>197</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C94" s="39"/>
-    </row>
-    <row r="95" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="C95" s="39"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
         <v>198</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B96" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C95" s="39"/>
-    </row>
-    <row r="96" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="C96" s="39"/>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>199</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B97" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C96" s="39"/>
-    </row>
-    <row r="97" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="C97" s="39"/>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
         <v>200</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B98" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C97" s="39"/>
-    </row>
-    <row r="98" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="C98" s="39"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
         <v>201</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C98" s="39"/>
-    </row>
-    <row r="99" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="C99" s="39"/>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
         <v>202</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C99" s="39"/>
-    </row>
-    <row r="100" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="C100" s="39"/>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
         <v>203</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C100" s="39"/>
-    </row>
-    <row r="101" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="C101" s="39"/>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
         <v>204</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C101" s="39"/>
-    </row>
-    <row r="102" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="C102" s="39"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
         <v>205</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C102" s="39"/>
-    </row>
-    <row r="103" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="C103" s="39"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
         <v>206</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C103" s="39"/>
-    </row>
-    <row r="104" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="C104" s="39"/>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
         <v>207</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C104" s="39"/>
-    </row>
-    <row r="105" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="C105" s="39"/>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C105" s="39"/>
-    </row>
-    <row r="106" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="C106" s="39"/>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
         <v>209</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B107" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C106" s="39"/>
-    </row>
-    <row r="107" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="C107" s="39"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
         <v>210</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="B108" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C107" s="39"/>
-    </row>
-    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="C108" s="39"/>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
         <v>211</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C108" s="39"/>
-    </row>
-    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="C109" s="39"/>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
         <v>212</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B110" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C109" s="39"/>
-    </row>
-    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="C110" s="39"/>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
         <v>213</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B111" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C110" s="39"/>
-    </row>
-    <row r="111" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="C111" s="39"/>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
         <v>214</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B112" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C111" s="39"/>
-    </row>
-    <row r="112" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="C112" s="39"/>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
         <v>215</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B113" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C112" s="39"/>
-    </row>
-    <row r="113" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="C113" s="39"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
         <v>216</v>
       </c>
-      <c r="B113" s="10" t="s">
+      <c r="B114" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C113" s="39"/>
-    </row>
-    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="C114" s="39"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
         <v>195</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C114" s="39"/>
-    </row>
-    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C115" s="39"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
         <v>194</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C115" s="39"/>
-    </row>
-    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="C116" s="39"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
         <v>193</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C116" s="39"/>
-    </row>
-    <row r="117" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="C117" s="39"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
         <v>192</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C117" s="39"/>
-    </row>
-    <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="C118" s="39"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
         <v>191</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C118" s="39"/>
-    </row>
-    <row r="119" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="C119" s="39"/>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
         <v>190</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C119" s="39"/>
-    </row>
-    <row r="120" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="C120" s="39"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
         <v>189</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C120" s="39"/>
-    </row>
-    <row r="121" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="C121" s="39"/>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
         <v>188</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C121" s="39"/>
+      <c r="C122" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C77:C85"/>
-    <mergeCell ref="C90:C121"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="C91:C122"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" location="actipass-variables" display="Please see ActiPASS output tables for more information where these variables are saved to." xr:uid="{F098AAF9-61B6-4AA4-94F5-D956F92B5131}"/>

</xml_diff>

<commit_message>
improved variable definition document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338638C6-6601-4941-A248-351FA7F32967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B969F1-AE03-40D0-95D3-A1BE2D7B446C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk160477595" localSheetId="0">Dictionary!$C$43</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="241">
   <si>
     <t>varNames</t>
   </si>
@@ -468,9 +471,6 @@
     <t>When a day has not enough walking, it affects the individual calibration (refrence-positions) and it can then lead to less accurate classifications</t>
   </si>
   <si>
-    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then it's a problem.</t>
-  </si>
-  <si>
     <t xml:space="preserve">A flag indicating if more than 30 minutes of "other" exist in the day </t>
   </si>
   <si>
@@ -483,19 +483,10 @@
     <t>A sleep-interval (a mid-point of a sleep interval to be precise) is not found within the day</t>
   </si>
   <si>
-    <t>This is not necessarily a problem. If the missing sleep is a technical problem, this day will then have much higher sedentary times than the other days</t>
-  </si>
-  <si>
     <t>Number of primary bedtimes (mid points) found within the current day</t>
   </si>
   <si>
     <t>Number of possible extra bedtimes found within the current day</t>
-  </si>
-  <si>
-    <t>Sleep algorithms is used only within these primary bedtimes</t>
-  </si>
-  <si>
-    <t>Slepp algorithm is not used for extra bedtimes</t>
   </si>
   <si>
     <t>Time of all upright activities/postures (i.e. Stand + Move + Walk + Run + Stair)</t>
@@ -784,30 +775,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The total time of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>possible sleep outside a bedtime</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> (this is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes.).</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
-  </si>
-  <si>
     <t>Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
   </si>
   <si>
@@ -1309,17 +1276,125 @@
     <t>The time within this calendar day which is flagged as belonging to a bedtime</t>
   </si>
   <si>
-    <t>This is same as "Sleep" now since ActiPASS version 1.50. Possible sleep outside bedtimes are now named "LieStill"</t>
-  </si>
-  <si>
     <t xml:space="preserve">A calendar day usually contains more than one (full or partial) bedtimes. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a bedtime. </t>
+  </si>
+  <si>
+    <r>
+      <t>“Sleep” is identifying in a process of two stages. During the first stage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, periods of most likely times-in-bed are identified by considering long continuous periods of lying-down</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and also prolonged periods of sitting to a lesser extent.  Then “Sleep” is defined as the total time of sleep detected within such times-in-bed periods according to ActiPASS sleep algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+1.	https://doi.org/10.3390/s21030904
+2.	https://doi.org/10.1111/jsr.13725</t>
+    </r>
+  </si>
+  <si>
+    <t>See definition of Sleep above</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The total time of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>possible sleep outside a bedtime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(not available under ProPASS mode)</t>
+    </r>
+  </si>
+  <si>
+    <t>This is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
+  </si>
+  <si>
+    <t>Lying down is detected using the algorithm described in      https://doi.org/10.3390/s21030904</t>
+  </si>
+  <si>
+    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then, an individual calibration error, an orientation error or other technical error could be the cause of this .</t>
+  </si>
+  <si>
+    <t>This is not necessarily a problem. this day will then have much higher sedentary times than the other days. Missing sleep could be due to other problems such as individual calibration or orientation issues</t>
+  </si>
+  <si>
+    <t>Sleep algorithms is used only within these primary bedtimes. See definition of sleep below.</t>
+  </si>
+  <si>
+    <t>Slepp algorithm is not used for extra bedtimes. See definition of sleep below.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1469,6 +1544,35 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1501,7 +1605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1599,6 +1703,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFABABAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1609,7 +1726,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1705,6 +1822,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1995,7 +2118,7 @@
   <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2019,7 +2142,7 @@
     </row>
     <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="A3" s="36" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -2046,13 +2169,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2063,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -2089,10 +2212,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
@@ -2100,18 +2223,18 @@
         <v>6</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
       <c r="B13" s="28" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
@@ -2120,7 +2243,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
@@ -2129,7 +2252,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2138,7 +2261,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
@@ -2147,18 +2270,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
@@ -2167,7 +2290,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>15</v>
@@ -2176,29 +2299,29 @@
     </row>
     <row r="21" spans="1:3" ht="30">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>98</v>
@@ -2209,57 +2332,57 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>100</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>105</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>108</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>109</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2268,7 +2391,7 @@
     </row>
     <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
       <c r="B30" s="29" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C30" s="15"/>
     </row>
@@ -2284,7 +2407,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>16</v>
@@ -2293,7 +2416,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>17</v>
@@ -2302,7 +2425,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>43</v>
@@ -2311,29 +2434,29 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>42</v>
@@ -2348,7 +2471,7 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>97</v>
@@ -2357,55 +2480,57 @@
     </row>
     <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="79.5">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="10" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="30">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>119</v>
+        <v>234</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>120</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
@@ -2416,25 +2541,27 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="C47" s="41" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="40"/>
     </row>
     <row r="49" spans="1:3" ht="30">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>28</v>
@@ -2443,7 +2570,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>23</v>
@@ -2452,7 +2579,7 @@
     </row>
     <row r="51" spans="1:3" ht="45">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>39</v>
@@ -2461,7 +2588,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>25</v>
@@ -2470,7 +2597,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>24</v>
@@ -2479,7 +2606,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>18</v>
@@ -2487,7 +2614,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>19</v>
@@ -2495,7 +2622,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>26</v>
@@ -2504,7 +2631,7 @@
     </row>
     <row r="57" spans="1:3" ht="30">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>40</v>
@@ -2513,7 +2640,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>27</v>
@@ -2522,22 +2649,22 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" ht="33" customHeight="1">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="5" customFormat="1">
@@ -2558,15 +2685,15 @@
         <v>7</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>86</v>
@@ -2574,10 +2701,10 @@
     </row>
     <row r="65" spans="1:3" ht="30">
       <c r="A65" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>87</v>
@@ -2585,10 +2712,10 @@
     </row>
     <row r="66" spans="1:3" ht="30">
       <c r="A66" s="24" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>88</v>
@@ -2596,10 +2723,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="24" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>92</v>
@@ -2607,10 +2734,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="24" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>93</v>
@@ -2618,10 +2745,10 @@
     </row>
     <row r="69" spans="1:3" s="5" customFormat="1">
       <c r="A69" s="24" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>89</v>
@@ -2639,7 +2766,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>20</v>
@@ -2647,7 +2774,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>41</v>
@@ -2655,7 +2782,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>21</v>
@@ -2663,7 +2790,7 @@
     </row>
     <row r="77" spans="1:3" s="5" customFormat="1" ht="120">
       <c r="B77" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>46</v>
@@ -2676,7 +2803,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>34</v>
@@ -2685,7 +2812,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>29</v>
@@ -2694,7 +2821,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>30</v>
@@ -2703,7 +2830,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>31</v>
@@ -2712,7 +2839,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>35</v>
@@ -2721,7 +2848,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>32</v>
@@ -2730,7 +2857,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>33</v>
@@ -2739,7 +2866,7 @@
     </row>
     <row r="86" spans="1:3" ht="30">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>38</v>
@@ -2748,7 +2875,7 @@
     </row>
     <row r="89" spans="1:3" s="5" customFormat="1" ht="75">
       <c r="B89" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C89" s="21" t="s">
         <v>48</v>
@@ -2756,7 +2883,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>49</v>
@@ -2767,7 +2894,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>50</v>
@@ -2776,7 +2903,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>51</v>
@@ -2785,7 +2912,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>52</v>
@@ -2794,7 +2921,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>53</v>
@@ -2803,7 +2930,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>54</v>
@@ -2812,7 +2939,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>55</v>
@@ -2821,7 +2948,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>56</v>
@@ -2830,7 +2957,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>57</v>
@@ -2839,7 +2966,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>58</v>
@@ -2848,7 +2975,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>59</v>
@@ -2857,7 +2984,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>60</v>
@@ -2866,7 +2993,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>61</v>
@@ -2875,7 +3002,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>62</v>
@@ -2884,7 +3011,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>63</v>
@@ -2893,7 +3020,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>64</v>
@@ -2902,7 +3029,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>65</v>
@@ -2911,7 +3038,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>66</v>
@@ -2920,7 +3047,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B109" s="10" t="s">
         <v>67</v>
@@ -2929,7 +3056,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B110" s="10" t="s">
         <v>68</v>
@@ -2938,7 +3065,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>69</v>
@@ -2947,7 +3074,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>70</v>
@@ -2956,7 +3083,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>71</v>
@@ -2965,7 +3092,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>72</v>
@@ -2974,7 +3101,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>80</v>
@@ -2983,7 +3110,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>73</v>
@@ -2992,7 +3119,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>74</v>
@@ -3001,7 +3128,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>75</v>
@@ -3010,7 +3137,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>76</v>
@@ -3019,7 +3146,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>77</v>
@@ -3028,7 +3155,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>78</v>
@@ -3037,7 +3164,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Improvement to variable definition document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B969F1-AE03-40D0-95D3-A1BE2D7B446C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B19C0A-B867-4937-8A93-2D1E3BA4640E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="243">
   <si>
     <t>varNames</t>
   </si>
@@ -733,9 +733,6 @@
     </r>
   </si>
   <si>
-    <t>A sleep interval is theoretically defined as the time between the first sleep onset and the last awakening. Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">The  time </t>
     </r>
@@ -773,9 +770,6 @@
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
-  </si>
-  <si>
-    <t>Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
   </si>
   <si>
     <t xml:space="preserve">Whether the  is a work-day or a leisure day. </t>
@@ -1273,22 +1267,65 @@
     <t>Bedtime</t>
   </si>
   <si>
-    <t>The time within this calendar day which is flagged as belonging to a bedtime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A calendar day usually contains more than one (full or partial) bedtimes. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a bedtime. </t>
-  </si>
-  <si>
-    <r>
-      <t>“Sleep” is identifying in a process of two stages. During the first stage</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
+    <t>See definition of Sleep above</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The total time of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>possible sleep outside a bedtime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(not available under ProPASS mode)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lying down is detected using the algorithm described in      https://doi.org/10.3390/s21030904</t>
+  </si>
+  <si>
+    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then, an individual calibration error, an orientation error or other technical error could be the cause of this .</t>
+  </si>
+  <si>
+    <t>This is not necessarily a problem. this day will then have much higher sedentary times than the other days. Missing sleep could be due to other problems such as individual calibration or orientation issues</t>
+  </si>
+  <si>
+    <t>Sleep algorithms is used only within these primary bedtimes. See definition of sleep below.</t>
+  </si>
+  <si>
+    <t>Slepp algorithm is not used for extra bedtimes. See definition of sleep below.</t>
+  </si>
+  <si>
+    <t>The time within this calendar day which is flagged as belonging to a times-in-bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sleep interval is theoretically defined as the time between the first sleep onset (see below for "Sleep") and the last awakening within each times-in-bed (see "Bedtime" above). Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval. </t>
+  </si>
+  <si>
+    <t>A calendar day usually contains more than one (full or partial) times-in-bed. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to most probable times-in-bed which are identified by considering long continuous periods of lying-down and also prolonged periods of sitting to a lesser extent.
+https://doi.org/10.3390/s21030904</t>
+  </si>
+  <si>
+    <r>
+      <t>“Sleep” is identified in a process of two stages.</t>
     </r>
     <r>
       <rPr>
@@ -1297,7 +1334,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>, periods of most likely times-in-bed are identified by considering long continuous periods of lying-down</t>
+      <t xml:space="preserve">  First periods of times-in-bed are identified (see above). Then “Sleep” is defined as the total time of sleep detected within such times-in-bed periods according to ActiPASS sleep algorithm</t>
     </r>
     <r>
       <rPr>
@@ -1307,25 +1344,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and also prolonged periods of sitting to a lesser extent.  Then “Sleep” is defined as the total time of sleep detected within such times-in-bed periods according to ActiPASS sleep algorithm</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>2</t>
     </r>
     <r>
@@ -1335,66 +1353,27 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-1.	https://doi.org/10.3390/s21030904
-2.	https://doi.org/10.1111/jsr.13725</t>
-    </r>
-  </si>
-  <si>
-    <t>See definition of Sleep above</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The total time of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>possible sleep outside a bedtime</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(not available under ProPASS mode)</t>
-    </r>
-  </si>
-  <si>
-    <t>This is found using running ActiPASS sleep algorithm on bouts of lying episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
-  </si>
-  <si>
-    <t>Lying down is detected using the algorithm described in      https://doi.org/10.3390/s21030904</t>
-  </si>
-  <si>
-    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then, an individual calibration error, an orientation error or other technical error could be the cause of this .</t>
-  </si>
-  <si>
-    <t>This is not necessarily a problem. this day will then have much higher sedentary times than the other days. Missing sleep could be due to other problems such as individual calibration or orientation issues</t>
-  </si>
-  <si>
-    <t>Sleep algorithms is used only within these primary bedtimes. See definition of sleep below.</t>
-  </si>
-  <si>
-    <t>Slepp algorithm is not used for extra bedtimes. See definition of sleep below.</t>
+https://doi.org/10.1111/jsr.13725</t>
+    </r>
+  </si>
+  <si>
+    <t>These behaviours are derived according to Acti4 algorithm:  https://doi.org/10.1123/jpah.2011-0347</t>
+  </si>
+  <si>
+    <t>Based on Acti4</t>
+  </si>
+  <si>
+    <t>Based on Acti4. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
+  </si>
+  <si>
+    <t>This is found using running ActiPASS sleep algorithm on bouts of lying (see "Lying" below) episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1566,12 +1545,6 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1814,6 +1787,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1823,10 +1799,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2142,7 +2115,7 @@
     </row>
     <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
       <c r="A3" s="36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -2172,10 +2145,10 @@
         <v>107</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2186,7 +2159,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -2212,10 +2185,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
@@ -2223,18 +2196,18 @@
         <v>6</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
       <c r="B13" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
@@ -2243,7 +2216,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
@@ -2252,7 +2225,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2261,7 +2234,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
@@ -2270,18 +2243,18 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>14</v>
@@ -2290,7 +2263,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>15</v>
@@ -2299,29 +2272,29 @@
     </row>
     <row r="21" spans="1:3" ht="30">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>98</v>
@@ -2332,18 +2305,18 @@
     </row>
     <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>101</v>
@@ -2354,35 +2327,35 @@
     </row>
     <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>104</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>105</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2391,7 +2364,7 @@
     </row>
     <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
       <c r="B30" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C30" s="15"/>
     </row>
@@ -2407,7 +2380,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>16</v>
@@ -2416,7 +2389,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>17</v>
@@ -2425,7 +2398,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>43</v>
@@ -2434,29 +2407,29 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>111</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>112</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>42</v>
@@ -2471,66 +2444,66 @@
     </row>
     <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="60">
       <c r="A41" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="45">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="79.5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="47.25">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
@@ -2541,27 +2514,27 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="41" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="40"/>
+      <c r="C48" s="37"/>
     </row>
     <row r="49" spans="1:3" ht="30">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>28</v>
@@ -2570,101 +2543,123 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="4"/>
+      <c r="C50" s="10" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="45">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="4"/>
+      <c r="C51" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C54" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C55" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="4"/>
+      <c r="C56" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="57" spans="1:3" ht="30">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="4"/>
+      <c r="C57" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C58" s="4"/>
+      <c r="C58" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="4"/>
+      <c r="C59" s="10" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="33" customHeight="1">
       <c r="A60" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>115</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="5" customFormat="1">
@@ -2690,10 +2685,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>86</v>
@@ -2701,10 +2696,10 @@
     </row>
     <row r="65" spans="1:3" ht="30">
       <c r="A65" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>87</v>
@@ -2712,10 +2707,10 @@
     </row>
     <row r="66" spans="1:3" ht="30">
       <c r="A66" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>88</v>
@@ -2723,10 +2718,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>92</v>
@@ -2734,10 +2729,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>93</v>
@@ -2745,10 +2740,10 @@
     </row>
     <row r="69" spans="1:3" s="5" customFormat="1">
       <c r="A69" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>89</v>
@@ -2766,7 +2761,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>20</v>
@@ -2774,7 +2769,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>41</v>
@@ -2782,7 +2777,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>21</v>
@@ -2797,81 +2792,81 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="38" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C79" s="38"/>
+      <c r="C79" s="39"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C80" s="38"/>
+      <c r="C80" s="39"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="38"/>
+      <c r="C81" s="39"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C82" s="38"/>
+      <c r="C82" s="39"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="38"/>
+      <c r="C83" s="39"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="38"/>
+      <c r="C84" s="39"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="38"/>
+      <c r="C85" s="39"/>
     </row>
     <row r="86" spans="1:3" ht="30">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="38"/>
+      <c r="C86" s="39"/>
     </row>
     <row r="89" spans="1:3" s="5" customFormat="1" ht="75">
       <c r="B89" s="20" t="s">
@@ -2883,299 +2878,300 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="39" t="s">
+      <c r="C91" s="40" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="39"/>
+      <c r="C92" s="40"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="39"/>
+      <c r="C93" s="40"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C94" s="39"/>
+      <c r="C94" s="40"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="39"/>
+      <c r="C95" s="40"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C96" s="39"/>
+      <c r="C96" s="40"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="39"/>
+      <c r="C97" s="40"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="39"/>
+      <c r="C98" s="40"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C99" s="39"/>
+      <c r="C99" s="40"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C100" s="39"/>
+      <c r="C100" s="40"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="39"/>
+      <c r="C101" s="40"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C102" s="39"/>
+      <c r="C102" s="40"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C103" s="39"/>
+      <c r="C103" s="40"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C104" s="39"/>
+      <c r="C104" s="40"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="39"/>
+      <c r="C105" s="40"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C106" s="39"/>
+      <c r="C106" s="40"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="39"/>
+      <c r="C107" s="40"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C108" s="39"/>
+      <c r="C108" s="40"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B109" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C109" s="39"/>
+      <c r="C109" s="40"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B110" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="39"/>
+      <c r="C110" s="40"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="39"/>
+      <c r="C111" s="40"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C112" s="39"/>
+      <c r="C112" s="40"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="39"/>
+      <c r="C113" s="40"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B114" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="39"/>
+      <c r="C114" s="40"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C115" s="39"/>
+      <c r="C115" s="40"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C116" s="39"/>
+      <c r="C116" s="40"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="39"/>
+      <c r="C117" s="40"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C118" s="39"/>
+      <c r="C118" s="40"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C119" s="39"/>
+      <c r="C119" s="40"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C120" s="39"/>
+      <c r="C120" s="40"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C121" s="39"/>
+      <c r="C121" s="40"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C122" s="39"/>
+      <c r="C122" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C78:C86"/>
     <mergeCell ref="C91:C122"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" location="actipass-variables" display="Please see ActiPASS output tables for more information where these variables are saved to." xr:uid="{F098AAF9-61B6-4AA4-94F5-D956F92B5131}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Improvements to variable definitions document
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B19C0A-B867-4937-8A93-2D1E3BA4640E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4657E9A-1608-4516-A34B-96C8CDB01B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,8 +1320,19 @@
     <t xml:space="preserve">A sleep interval is theoretically defined as the time between the first sleep onset (see below for "Sleep") and the last awakening within each times-in-bed (see "Bedtime" above). Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval. </t>
   </si>
   <si>
-    <t>A calendar day usually contains more than one (full or partial) times-in-bed. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to most probable times-in-bed which are identified by considering long continuous periods of lying-down and also prolonged periods of sitting to a lesser extent.
-https://doi.org/10.3390/s21030904</t>
+    <t>These behaviours are derived according to Acti4 algorithm:  https://doi.org/10.1123/jpah.2011-0347</t>
+  </si>
+  <si>
+    <t>Based on Acti4</t>
+  </si>
+  <si>
+    <t>Based on Acti4. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
+  </si>
+  <si>
+    <t>A calendar day usually contains more than one (full or partial) times-in-bed. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to most probable times-in-bed which are identified by considering long continuous periods of lying-down (see "Lie" below) and also prolonged periods of sitting to a lesser extent.</t>
+  </si>
+  <si>
+    <t>This is found using running ActiPASS sleep algorithm on bouts of lying (see "Lie" below) episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
   </si>
   <si>
     <r>
@@ -1334,7 +1345,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">  First periods of times-in-bed are identified (see above). Then “Sleep” is defined as the total time of sleep detected within such times-in-bed periods according to ActiPASS sleep algorithm</t>
+      <t xml:space="preserve">  First periods of times-in-bed are identified (see above). Then “Sleep” is defined as the total time of sleep detected within such periods of times-in-bed  according to ActiPASS sleep algorithm</t>
     </r>
     <r>
       <rPr>
@@ -1355,18 +1366,6 @@
       <t xml:space="preserve">
 https://doi.org/10.1111/jsr.13725</t>
     </r>
-  </si>
-  <si>
-    <t>These behaviours are derived according to Acti4 algorithm:  https://doi.org/10.1123/jpah.2011-0347</t>
-  </si>
-  <si>
-    <t>Based on Acti4</t>
-  </si>
-  <si>
-    <t>Based on Acti4. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
-  </si>
-  <si>
-    <t>This is found using running ActiPASS sleep algorithm on bouts of lying (see "Lying" below) episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
   </si>
 </sst>
 </file>
@@ -1790,6 +1789,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1798,9 +1800,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2451,7 +2450,7 @@
       </c>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" ht="60">
+    <row r="41" spans="1:3" ht="45">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>235</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="45">
@@ -2481,7 +2480,7 @@
         <v>95</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30">
@@ -2503,7 +2502,7 @@
         <v>229</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
@@ -2519,7 +2518,7 @@
       <c r="B47" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="38" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2549,7 +2548,7 @@
         <v>23</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="45">
@@ -2560,7 +2559,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2571,7 +2570,7 @@
         <v>25</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2582,7 +2581,7 @@
         <v>24</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2593,7 +2592,7 @@
         <v>18</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2604,7 +2603,7 @@
         <v>19</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2615,7 +2614,7 @@
         <v>26</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="30">
@@ -2626,7 +2625,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2637,7 +2636,7 @@
         <v>27</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2648,7 +2647,7 @@
         <v>106</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="33" customHeight="1">
@@ -2659,7 +2658,7 @@
         <v>226</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="5" customFormat="1">
@@ -2792,7 +2791,7 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2803,7 +2802,7 @@
       <c r="B79" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C79" s="39"/>
+      <c r="C79" s="40"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
@@ -2812,7 +2811,7 @@
       <c r="B80" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C80" s="39"/>
+      <c r="C80" s="40"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
@@ -2821,7 +2820,7 @@
       <c r="B81" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="39"/>
+      <c r="C81" s="40"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
@@ -2830,7 +2829,7 @@
       <c r="B82" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C82" s="39"/>
+      <c r="C82" s="40"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
@@ -2839,7 +2838,7 @@
       <c r="B83" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="39"/>
+      <c r="C83" s="40"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
@@ -2848,7 +2847,7 @@
       <c r="B84" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="39"/>
+      <c r="C84" s="40"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
@@ -2857,7 +2856,7 @@
       <c r="B85" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="39"/>
+      <c r="C85" s="40"/>
     </row>
     <row r="86" spans="1:3" ht="30">
       <c r="A86" t="s">
@@ -2866,7 +2865,7 @@
       <c r="B86" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="39"/>
+      <c r="C86" s="40"/>
     </row>
     <row r="89" spans="1:3" s="5" customFormat="1" ht="75">
       <c r="B89" s="20" t="s">
@@ -2883,7 +2882,7 @@
       <c r="B91" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="40" t="s">
+      <c r="C91" s="41" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2894,7 +2893,7 @@
       <c r="B92" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="40"/>
+      <c r="C92" s="41"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
@@ -2903,7 +2902,7 @@
       <c r="B93" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="40"/>
+      <c r="C93" s="41"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
@@ -2912,7 +2911,7 @@
       <c r="B94" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C94" s="40"/>
+      <c r="C94" s="41"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
@@ -2921,7 +2920,7 @@
       <c r="B95" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="40"/>
+      <c r="C95" s="41"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
@@ -2930,7 +2929,7 @@
       <c r="B96" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C96" s="40"/>
+      <c r="C96" s="41"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
@@ -2939,7 +2938,7 @@
       <c r="B97" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="40"/>
+      <c r="C97" s="41"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
@@ -2948,7 +2947,7 @@
       <c r="B98" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="40"/>
+      <c r="C98" s="41"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
@@ -2957,7 +2956,7 @@
       <c r="B99" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C99" s="40"/>
+      <c r="C99" s="41"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
@@ -2966,7 +2965,7 @@
       <c r="B100" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C100" s="40"/>
+      <c r="C100" s="41"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
@@ -2975,7 +2974,7 @@
       <c r="B101" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="40"/>
+      <c r="C101" s="41"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
@@ -2984,7 +2983,7 @@
       <c r="B102" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C102" s="40"/>
+      <c r="C102" s="41"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
@@ -2993,7 +2992,7 @@
       <c r="B103" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C103" s="40"/>
+      <c r="C103" s="41"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
@@ -3002,7 +3001,7 @@
       <c r="B104" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C104" s="40"/>
+      <c r="C104" s="41"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
@@ -3011,7 +3010,7 @@
       <c r="B105" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="40"/>
+      <c r="C105" s="41"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
@@ -3020,7 +3019,7 @@
       <c r="B106" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C106" s="40"/>
+      <c r="C106" s="41"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
@@ -3029,7 +3028,7 @@
       <c r="B107" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="40"/>
+      <c r="C107" s="41"/>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
@@ -3038,7 +3037,7 @@
       <c r="B108" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C108" s="40"/>
+      <c r="C108" s="41"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
@@ -3047,7 +3046,7 @@
       <c r="B109" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C109" s="40"/>
+      <c r="C109" s="41"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
@@ -3056,7 +3055,7 @@
       <c r="B110" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="40"/>
+      <c r="C110" s="41"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
@@ -3065,7 +3064,7 @@
       <c r="B111" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="40"/>
+      <c r="C111" s="41"/>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
@@ -3074,7 +3073,7 @@
       <c r="B112" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C112" s="40"/>
+      <c r="C112" s="41"/>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
@@ -3083,7 +3082,7 @@
       <c r="B113" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="40"/>
+      <c r="C113" s="41"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
@@ -3092,7 +3091,7 @@
       <c r="B114" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="40"/>
+      <c r="C114" s="41"/>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
@@ -3101,7 +3100,7 @@
       <c r="B115" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C115" s="40"/>
+      <c r="C115" s="41"/>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
@@ -3110,7 +3109,7 @@
       <c r="B116" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C116" s="40"/>
+      <c r="C116" s="41"/>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
@@ -3119,7 +3118,7 @@
       <c r="B117" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="40"/>
+      <c r="C117" s="41"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
@@ -3128,7 +3127,7 @@
       <c r="B118" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C118" s="40"/>
+      <c r="C118" s="41"/>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
@@ -3137,7 +3136,7 @@
       <c r="B119" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C119" s="40"/>
+      <c r="C119" s="41"/>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
@@ -3146,7 +3145,7 @@
       <c r="B120" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C120" s="40"/>
+      <c r="C120" s="41"/>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
@@ -3155,7 +3154,7 @@
       <c r="B121" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C121" s="40"/>
+      <c r="C121" s="41"/>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
@@ -3164,7 +3163,7 @@
       <c r="B122" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C122" s="40"/>
+      <c r="C122" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added definition for "RefPosInfo"
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
+++ b/docs/Extra/ActiPASS_Variable-definitions_NewFormat_ActiPASS_Version_1.50.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4657E9A-1608-4516-A34B-96C8CDB01B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D09A24-2465-463B-95B4-9AA79042197F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk160477595" localSheetId="0">Dictionary!$C$43</definedName>
+    <definedName name="_Hlk160477595" localSheetId="0">Dictionary!$C$44</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="245">
   <si>
     <t>varNames</t>
   </si>
@@ -1078,6 +1078,208 @@
     <t xml:space="preserve">Following variables are derived daily. A day is a calendar day starting from 00:00:00 and ending with 23:59:59. The first and last day could be partial days. </t>
   </si>
   <si>
+    <t>A day can be further sub-divided into domains such as 'Work' and 'Leisure' and following variables can be generated for each such sub-domain within a calendar day.  Such variables will be prefixed with the domain (Ex. Work_Duration) This additional domain specific data is available only when the additional diary containing such data is included in ActiPASS processing, and also the relevant domain names are specified under "Stat Domains" options before stats generation.</t>
+  </si>
+  <si>
+    <t>example "2022-03-28 15.12.34"</t>
+  </si>
+  <si>
+    <t>Follow this link for more information regarding how these variables are saved to ActiPASS output tables (CSV files)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A flag indicating if the day has not enough wear time (20 hrs). </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Should always be zero for the table </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ProPASS_WideFormat_MasterFile.csv"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The auto detected quality check flag for the day. possible values: "OK", "Check" or "NotOK" </t>
+  </si>
+  <si>
+    <r>
+      <t>ProPASS wide-format table (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"ProPASS_WideFormat_MasterFile.csv"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>) contains days only days where this flag is "OK"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> not a part of Awake </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>variable below</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>not a part of SleepInterval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> below</t>
+    </r>
+  </si>
+  <si>
+    <t>Time of activities in "Other" postures/activities with movements which cannot be classified into known activities/postures</t>
+  </si>
+  <si>
+    <t>Bedtime</t>
+  </si>
+  <si>
+    <t>See definition of Sleep above</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The total time of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>possible sleep outside a bedtime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(not available under ProPASS mode)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lying down is detected using the algorithm described in      https://doi.org/10.3390/s21030904</t>
+  </si>
+  <si>
+    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then, an individual calibration error, an orientation error or other technical error could be the cause of this .</t>
+  </si>
+  <si>
+    <t>This is not necessarily a problem. this day will then have much higher sedentary times than the other days. Missing sleep could be due to other problems such as individual calibration or orientation issues</t>
+  </si>
+  <si>
+    <t>Sleep algorithms is used only within these primary bedtimes. See definition of sleep below.</t>
+  </si>
+  <si>
+    <t>Slepp algorithm is not used for extra bedtimes. See definition of sleep below.</t>
+  </si>
+  <si>
+    <t>The time within this calendar day which is flagged as belonging to a times-in-bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sleep interval is theoretically defined as the time between the first sleep onset (see below for "Sleep") and the last awakening within each times-in-bed (see "Bedtime" above). Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval. </t>
+  </si>
+  <si>
+    <t>These behaviours are derived according to Acti4 algorithm:  https://doi.org/10.1123/jpah.2011-0347</t>
+  </si>
+  <si>
+    <t>Based on Acti4</t>
+  </si>
+  <si>
+    <t>Based on Acti4. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
+  </si>
+  <si>
+    <t>A calendar day usually contains more than one (full or partial) times-in-bed. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to most probable times-in-bed which are identified by considering long continuous periods of lying-down (see "Lie" below) and also prolonged periods of sitting to a lesser extent.</t>
+  </si>
+  <si>
+    <t>This is found using running ActiPASS sleep algorithm on bouts of lying (see "Lie" below) episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
+  </si>
+  <si>
+    <r>
+      <t>“Sleep” is identified in a process of two stages.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  First periods of times-in-bed are identified (see above). Then “Sleep” is defined as the total time of sleep detected within such periods of times-in-bed  according to ActiPASS sleep algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+https://doi.org/10.1111/jsr.13725</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1161,218 +1363,22 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-    Only days determined to be valid (see below) are listed in the table.
-    Each variable is suffixed with day number. For example the suffix  "_1" in "Date_1" indicates the day number 1. </t>
-    </r>
-  </si>
-  <si>
-    <t>A day can be further sub-divided into domains such as 'Work' and 'Leisure' and following variables can be generated for each such sub-domain within a calendar day.  Such variables will be prefixed with the domain (Ex. Work_Duration) This additional domain specific data is available only when the additional diary containing such data is included in ActiPASS processing, and also the relevant domain names are specified under "Stat Domains" options before stats generation.</t>
-  </si>
-  <si>
-    <t>example "2022-03-28 15.12.34"</t>
-  </si>
-  <si>
-    <t>Follow this link for more information regarding how these variables are saved to ActiPASS output tables (CSV files)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A flag indicating if the day has not enough wear time (20 hrs). </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Should always be zero for the table </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"ProPASS_WideFormat_MasterFile.csv"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The auto detected quality check flag for the day. possible values: "OK", "Check" or "NotOK" </t>
-  </si>
-  <si>
-    <r>
-      <t>ProPASS wide-format table (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"ProPASS_WideFormat_MasterFile.csv"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>) contains days only days where this flag is "OK"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> not a part of Awake </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>variable below</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There could be more than one sleep-intervals happening for a given calendar day. It's important to highlight that this time is </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>not a part of SleepInterval</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> below</t>
-    </r>
-  </si>
-  <si>
-    <t>Time of activities in "Other" postures/activities with movements which cannot be classified into known activities/postures</t>
-  </si>
-  <si>
-    <t>Bedtime</t>
-  </si>
-  <si>
-    <t>See definition of Sleep above</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The total time of </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>possible sleep outside a bedtime</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(not available under ProPASS mode)</t>
-    </r>
-  </si>
-  <si>
-    <t>Lying down is detected using the algorithm described in      https://doi.org/10.3390/s21030904</t>
-  </si>
-  <si>
-    <t>Too much other itself is not necessarily a problem. Those times can be actual activities/scenarios which are not dtected by ActiPASS. However if it is combined with no-walking or no standing then, an individual calibration error, an orientation error or other technical error could be the cause of this .</t>
-  </si>
-  <si>
-    <t>This is not necessarily a problem. this day will then have much higher sedentary times than the other days. Missing sleep could be due to other problems such as individual calibration or orientation issues</t>
-  </si>
-  <si>
-    <t>Sleep algorithms is used only within these primary bedtimes. See definition of sleep below.</t>
-  </si>
-  <si>
-    <t>Slepp algorithm is not used for extra bedtimes. See definition of sleep below.</t>
-  </si>
-  <si>
-    <t>The time within this calendar day which is flagged as belonging to a times-in-bed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A sleep interval is theoretically defined as the time between the first sleep onset (see below for "Sleep") and the last awakening within each times-in-bed (see "Bedtime" above). Therefore, a calendar day usually contains more than one (full or partial) sleep-intervals. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to a sleep-interval. </t>
-  </si>
-  <si>
-    <t>These behaviours are derived according to Acti4 algorithm:  https://doi.org/10.1123/jpah.2011-0347</t>
-  </si>
-  <si>
-    <t>Based on Acti4</t>
-  </si>
-  <si>
-    <t>Based on Acti4. Time of 'Other' could be high due to various reasons such as: actual activities such gym equipment, rowing/kayaking or individual calibration issues.</t>
-  </si>
-  <si>
-    <t>A calendar day usually contains more than one (full or partial) times-in-bed. This variable is calculated by counting the number of epochs (1s) which are flagged as belonging to most probable times-in-bed which are identified by considering long continuous periods of lying-down (see "Lie" below) and also prolonged periods of sitting to a lesser extent.</t>
-  </si>
-  <si>
-    <t>This is found using running ActiPASS sleep algorithm on bouts of lying (see "Lie" below) episodes outside bedtimes. In ActiPASS versions prior to 1.50 this was called "SleepOutBed"</t>
-  </si>
-  <si>
-    <r>
-      <t>“Sleep” is identified in a process of two stages.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  First periods of times-in-bed are identified (see above). Then “Sleep” is defined as the total time of sleep detected within such periods of times-in-bed  according to ActiPASS sleep algorithm</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-https://doi.org/10.1111/jsr.13725</t>
-    </r>
+      Only days determined to be valid (see below) are listed.
+      Each variable is suffixed with day number. For example the suffix  "_1" in "Date_1" indicates the day number 1. </t>
+    </r>
+  </si>
+  <si>
+    <t>RefPosInfo</t>
+  </si>
+  <si>
+    <t>Automatic individual calibration angles (in degrees) for this day. Given as absolute inclination and forward backward inclination of thigh at the reference-position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2087,40 +2093,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="79" style="3" customWidth="1"/>
     <col min="3" max="3" width="154.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="26" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:3" s="26" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
     </row>
-    <row r="2" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
+    <row r="2" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
     </row>
-    <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1">
+    <row r="3" spans="1:3" s="26" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickTop="1"/>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1">
+    <row r="4" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30.75" thickTop="1">
+    <row r="6" spans="1:3" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2139,7 +2145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -2150,7 +2156,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2158,10 +2164,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2170,7 +2176,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2179,7 +2185,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="11" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" ht="30">
+    <row r="12" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
@@ -2201,19 +2207,19 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1">
+    <row r="13" spans="1:3" s="17" customFormat="1" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28" t="s">
         <v>215</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="33" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -2222,7 +2228,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -2231,7 +2237,7 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -2240,7 +2246,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -2260,7 +2266,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -2269,906 +2275,915 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C21" s="10" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30">
-      <c r="A26" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="10" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" s="14" customFormat="1" ht="90">
-      <c r="B30" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:3" s="14" customFormat="1">
-      <c r="B31" s="16"/>
-      <c r="C31" s="15"/>
-    </row>
-    <row r="32" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B32" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="C42" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="37"/>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B39" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" ht="30">
-      <c r="A40" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" ht="45">
-      <c r="A41" t="s">
-        <v>227</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="45">
-      <c r="A42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="47.25">
-      <c r="A43" t="s">
-        <v>143</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30">
-      <c r="A44" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30">
-      <c r="A45" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B46" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A48" t="s">
-        <v>147</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="37"/>
-    </row>
-    <row r="49" spans="1:3" ht="30">
-      <c r="A49" t="s">
-        <v>148</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="45">
-      <c r="A51" t="s">
-        <v>150</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>151</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>152</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>153</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>154</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>155</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="30">
-      <c r="A57" t="s">
-        <v>156</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>157</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>158</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="33" customHeight="1">
-      <c r="A60" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="5" customFormat="1">
-      <c r="C61" s="19" t="s">
+    <row r="62" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1">
-      <c r="B62" s="19" t="s">
+    <row r="63" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="409.5" customHeight="1" thickBot="1">
-      <c r="A63" s="22" t="s">
+    <row r="64" spans="1:3" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="23" t="s">
+      <c r="B64" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C64" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="24" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B65" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C65" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30">
-      <c r="A65" s="24" t="s">
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B66" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C66" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30">
-      <c r="A66" s="24" t="s">
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B67" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="C67" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="24" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B68" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C68" s="25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="24" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B69" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C69" s="25" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1">
-      <c r="A69" s="24" t="s">
+    <row r="70" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="B69" s="25" t="s">
+      <c r="B70" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C70" s="25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1">
-      <c r="A70" s="24"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-    </row>
-    <row r="71" spans="1:3" s="5" customFormat="1">
-      <c r="B71" s="18" t="s">
+    <row r="71" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="24"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+    </row>
+    <row r="72" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>168</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>166</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="120">
-      <c r="B77" s="12" t="s">
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C78" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="C78" s="39" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B80" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C79" s="40"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+      <c r="C80" s="40"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>170</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B81" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C80" s="40"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+      <c r="C81" s="40"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>171</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="40"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
+      <c r="C82" s="40"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>172</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B83" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C82" s="40"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+      <c r="C83" s="40"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>173</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B84" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="40"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+      <c r="C84" s="40"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>174</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B85" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="40"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+      <c r="C85" s="40"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>175</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="40"/>
-    </row>
-    <row r="86" spans="1:3" ht="30">
-      <c r="A86" t="s">
+      <c r="C86" s="40"/>
+    </row>
+    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>176</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="40"/>
-    </row>
-    <row r="89" spans="1:3" s="5" customFormat="1" ht="75">
-      <c r="B89" s="20" t="s">
+      <c r="C87" s="40"/>
+    </row>
+    <row r="90" spans="1:3" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B90" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C89" s="21" t="s">
+      <c r="C90" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>177</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B92" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="41" t="s">
+      <c r="C92" s="41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>178</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B93" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="41"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
+      <c r="C93" s="41"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>179</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B94" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="41"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+      <c r="C94" s="41"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>188</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B95" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C94" s="41"/>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
+      <c r="C95" s="41"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>189</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B96" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C95" s="41"/>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+      <c r="C96" s="41"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B97" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C96" s="41"/>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+      <c r="C97" s="41"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>191</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B98" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C97" s="41"/>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
+      <c r="C98" s="41"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>192</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B99" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="41"/>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
+      <c r="C99" s="41"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>193</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C99" s="41"/>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
+      <c r="C100" s="41"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>194</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C100" s="41"/>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
+      <c r="C101" s="41"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>195</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="41"/>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
+      <c r="C102" s="41"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>196</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C102" s="41"/>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
+      <c r="C103" s="41"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>197</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C103" s="41"/>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
+      <c r="C104" s="41"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>198</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C104" s="41"/>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
+      <c r="C105" s="41"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>199</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="41"/>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
+      <c r="C106" s="41"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>200</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C106" s="41"/>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
+      <c r="C107" s="41"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>201</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="B108" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="41"/>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
+      <c r="C108" s="41"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>202</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B109" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C108" s="41"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
+      <c r="C109" s="41"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>203</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B110" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C109" s="41"/>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
+      <c r="C110" s="41"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>204</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B111" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="41"/>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
+      <c r="C111" s="41"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>205</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B112" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="41"/>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
+      <c r="C112" s="41"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>206</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="B113" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C112" s="41"/>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
+      <c r="C113" s="41"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>207</v>
       </c>
-      <c r="B113" s="10" t="s">
+      <c r="B114" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="41"/>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
+      <c r="C114" s="41"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>208</v>
       </c>
-      <c r="B114" s="10" t="s">
+      <c r="B115" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="41"/>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
+      <c r="C115" s="41"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>187</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C115" s="41"/>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
+      <c r="C116" s="41"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>186</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C116" s="41"/>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
+      <c r="C117" s="41"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>185</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="41"/>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
+      <c r="C118" s="41"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>184</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C118" s="41"/>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
+      <c r="C119" s="41"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>183</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C119" s="41"/>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
+      <c r="C120" s="41"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>182</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C120" s="41"/>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
+      <c r="C121" s="41"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>181</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C121" s="41"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
+      <c r="C122" s="41"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>180</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C122" s="41"/>
+      <c r="C123" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="C91:C122"/>
+    <mergeCell ref="C79:C87"/>
+    <mergeCell ref="C92:C123"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>

</xml_diff>